<commit_message>
Copy latest linkml_model to root level
</commit_message>
<xml_diff>
--- a/linkml_model/excel/meta.xlsx
+++ b/linkml_model/excel/meta.xlsx
@@ -24,18 +24,21 @@
     <sheet name="anonymous_class_expression" sheetId="15" state="visible" r:id="rId15"/>
     <sheet name="class_definition" sheetId="16" state="visible" r:id="rId16"/>
     <sheet name="class_rule" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="pattern_expression" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="import_expression" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="setting" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="prefix" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="local_name" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="example" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="alt_description" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="permissible_value" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="unique_key" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="UnitOfMeasure" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="annotation" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="extension" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="array_expression" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="dimension_expression" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="pattern_expression" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="import_expression" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="setting" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="prefix" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="local_name" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="example" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="alt_description" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="permissible_value" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="unique_key" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="UnitOfMeasure" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="annotation" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="AnyValue" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="extension" sheetId="32" state="visible" r:id="rId32"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -957,7 +960,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BI1"/>
+  <dimension ref="A1:BJ1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1058,215 +1061,220 @@
       </c>
       <c r="S1" t="inlineStr">
         <is>
+          <t>exact_cardinality</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
           <t>minimum_cardinality</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>maximum_cardinality</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>has_member</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>all_members</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>none_of</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>exactly_one_of</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>any_of</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>all_of</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>extensions</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>annotations</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>alt_descriptions</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>deprecated</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>todos</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>comments</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>examples</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>in_subset</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>from_schema</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>imported_from</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>source</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>in_language</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>deprecated element has exact replacement</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>deprecated element has possible replacement</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>aliases</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>structured_aliases</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>mappings</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>exact mappings</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>close mappings</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>related mappings</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>narrow mappings</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>broad mappings</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>created_by</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>contributors</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>created_on</t>
         </is>
       </c>
-      <c r="BD1" t="inlineStr">
+      <c r="BE1" t="inlineStr">
         <is>
           <t>last_updated_on</t>
         </is>
       </c>
-      <c r="BE1" t="inlineStr">
+      <c r="BF1" t="inlineStr">
         <is>
           <t>modified_by</t>
         </is>
       </c>
-      <c r="BF1" t="inlineStr">
+      <c r="BG1" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
-      <c r="BG1" t="inlineStr">
+      <c r="BH1" t="inlineStr">
         <is>
           <t>rank</t>
         </is>
       </c>
-      <c r="BH1" t="inlineStr">
+      <c r="BI1" t="inlineStr">
         <is>
           <t>categories</t>
         </is>
       </c>
-      <c r="BI1" t="inlineStr">
+      <c r="BJ1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
@@ -1288,7 +1296,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DH1"/>
+  <dimension ref="A1:DK1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1319,540 +1327,555 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>array</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>inherited</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>readonly</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>ifabsent</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>list_elements_unique</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>list_elements_ordered</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>shared</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>key</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>designates_type</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>alias</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>owner</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>domain_of</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>subproperty_of</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>symmetric</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>reflexive</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>locally_reflexive</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>irreflexive</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>asymmetric</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>transitive</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>inverse</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>is_class_field</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>transitive_form_of</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>reflexive_transitive_form_of</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>role</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>is_usage_slot</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>usage_slot_name</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>relational_role</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>slot_group</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>is_grouping_slot</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>path_rule</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>disjoint_with</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>children_are_mutually_disjoint</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>union_of</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>range</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>range_expression</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>enum_range</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>required</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>recommended</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>inlined</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>inlined_as_list</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>minimum_value</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>maximum_value</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>pattern</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>structured_pattern</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>unit</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>implicit_prefix</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>value_presence</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>equals_string</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>equals_string_in</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>equals_number</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>equals_expression</t>
         </is>
       </c>
-      <c r="BD1" t="inlineStr">
+      <c r="BE1" t="inlineStr">
+        <is>
+          <t>exact_cardinality</t>
+        </is>
+      </c>
+      <c r="BF1" t="inlineStr">
         <is>
           <t>minimum_cardinality</t>
         </is>
       </c>
-      <c r="BE1" t="inlineStr">
+      <c r="BG1" t="inlineStr">
         <is>
           <t>maximum_cardinality</t>
         </is>
       </c>
-      <c r="BF1" t="inlineStr">
+      <c r="BH1" t="inlineStr">
         <is>
           <t>has_member</t>
         </is>
       </c>
-      <c r="BG1" t="inlineStr">
+      <c r="BI1" t="inlineStr">
         <is>
           <t>all_members</t>
         </is>
       </c>
-      <c r="BH1" t="inlineStr">
+      <c r="BJ1" t="inlineStr">
         <is>
           <t>none_of</t>
         </is>
       </c>
-      <c r="BI1" t="inlineStr">
+      <c r="BK1" t="inlineStr">
         <is>
           <t>exactly_one_of</t>
         </is>
       </c>
-      <c r="BJ1" t="inlineStr">
+      <c r="BL1" t="inlineStr">
         <is>
           <t>any_of</t>
         </is>
       </c>
-      <c r="BK1" t="inlineStr">
+      <c r="BM1" t="inlineStr">
         <is>
           <t>all_of</t>
         </is>
       </c>
-      <c r="BL1" t="inlineStr">
+      <c r="BN1" t="inlineStr">
         <is>
           <t>is_a</t>
         </is>
       </c>
-      <c r="BM1" t="inlineStr">
+      <c r="BO1" t="inlineStr">
         <is>
           <t>abstract</t>
         </is>
       </c>
-      <c r="BN1" t="inlineStr">
+      <c r="BP1" t="inlineStr">
         <is>
           <t>mixin</t>
         </is>
       </c>
-      <c r="BO1" t="inlineStr">
+      <c r="BQ1" t="inlineStr">
         <is>
           <t>mixins</t>
         </is>
       </c>
-      <c r="BP1" t="inlineStr">
+      <c r="BR1" t="inlineStr">
         <is>
           <t>apply_to</t>
         </is>
       </c>
-      <c r="BQ1" t="inlineStr">
+      <c r="BS1" t="inlineStr">
         <is>
           <t>values_from</t>
         </is>
       </c>
-      <c r="BR1" t="inlineStr">
+      <c r="BT1" t="inlineStr">
         <is>
           <t>string_serialization</t>
         </is>
       </c>
-      <c r="BS1" t="inlineStr">
+      <c r="BU1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="BT1" t="inlineStr">
+      <c r="BV1" t="inlineStr">
         <is>
           <t>id_prefixes</t>
         </is>
       </c>
-      <c r="BU1" t="inlineStr">
+      <c r="BW1" t="inlineStr">
+        <is>
+          <t>id_prefixes_are_closed</t>
+        </is>
+      </c>
+      <c r="BX1" t="inlineStr">
         <is>
           <t>definition_uri</t>
         </is>
       </c>
-      <c r="BV1" t="inlineStr">
+      <c r="BY1" t="inlineStr">
         <is>
           <t>local_names</t>
         </is>
       </c>
-      <c r="BW1" t="inlineStr">
+      <c r="BZ1" t="inlineStr">
         <is>
           <t>conforms_to</t>
         </is>
       </c>
-      <c r="BX1" t="inlineStr">
+      <c r="CA1" t="inlineStr">
         <is>
           <t>implements</t>
         </is>
       </c>
-      <c r="BY1" t="inlineStr">
+      <c r="CB1" t="inlineStr">
         <is>
           <t>instantiates</t>
         </is>
       </c>
-      <c r="BZ1" t="inlineStr">
+      <c r="CC1" t="inlineStr">
         <is>
           <t>extensions</t>
         </is>
       </c>
-      <c r="CA1" t="inlineStr">
+      <c r="CD1" t="inlineStr">
         <is>
           <t>annotations</t>
         </is>
       </c>
-      <c r="CB1" t="inlineStr">
+      <c r="CE1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="CC1" t="inlineStr">
+      <c r="CF1" t="inlineStr">
         <is>
           <t>alt_descriptions</t>
         </is>
       </c>
-      <c r="CD1" t="inlineStr">
+      <c r="CG1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="CE1" t="inlineStr">
+      <c r="CH1" t="inlineStr">
         <is>
           <t>deprecated</t>
         </is>
       </c>
-      <c r="CF1" t="inlineStr">
+      <c r="CI1" t="inlineStr">
         <is>
           <t>todos</t>
         </is>
       </c>
-      <c r="CG1" t="inlineStr">
+      <c r="CJ1" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
       </c>
-      <c r="CH1" t="inlineStr">
+      <c r="CK1" t="inlineStr">
         <is>
           <t>comments</t>
         </is>
       </c>
-      <c r="CI1" t="inlineStr">
+      <c r="CL1" t="inlineStr">
         <is>
           <t>examples</t>
         </is>
       </c>
-      <c r="CJ1" t="inlineStr">
+      <c r="CM1" t="inlineStr">
         <is>
           <t>in_subset</t>
         </is>
       </c>
-      <c r="CK1" t="inlineStr">
+      <c r="CN1" t="inlineStr">
         <is>
           <t>from_schema</t>
         </is>
       </c>
-      <c r="CL1" t="inlineStr">
+      <c r="CO1" t="inlineStr">
         <is>
           <t>imported_from</t>
         </is>
       </c>
-      <c r="CM1" t="inlineStr">
+      <c r="CP1" t="inlineStr">
         <is>
           <t>source</t>
         </is>
       </c>
-      <c r="CN1" t="inlineStr">
+      <c r="CQ1" t="inlineStr">
         <is>
           <t>in_language</t>
         </is>
       </c>
-      <c r="CO1" t="inlineStr">
+      <c r="CR1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="CP1" t="inlineStr">
+      <c r="CS1" t="inlineStr">
         <is>
           <t>deprecated element has exact replacement</t>
         </is>
       </c>
-      <c r="CQ1" t="inlineStr">
+      <c r="CT1" t="inlineStr">
         <is>
           <t>deprecated element has possible replacement</t>
         </is>
       </c>
-      <c r="CR1" t="inlineStr">
+      <c r="CU1" t="inlineStr">
         <is>
           <t>aliases</t>
         </is>
       </c>
-      <c r="CS1" t="inlineStr">
+      <c r="CV1" t="inlineStr">
         <is>
           <t>structured_aliases</t>
         </is>
       </c>
-      <c r="CT1" t="inlineStr">
+      <c r="CW1" t="inlineStr">
         <is>
           <t>mappings</t>
         </is>
       </c>
-      <c r="CU1" t="inlineStr">
+      <c r="CX1" t="inlineStr">
         <is>
           <t>exact mappings</t>
         </is>
       </c>
-      <c r="CV1" t="inlineStr">
+      <c r="CY1" t="inlineStr">
         <is>
           <t>close mappings</t>
         </is>
       </c>
-      <c r="CW1" t="inlineStr">
+      <c r="CZ1" t="inlineStr">
         <is>
           <t>related mappings</t>
         </is>
       </c>
-      <c r="CX1" t="inlineStr">
+      <c r="DA1" t="inlineStr">
         <is>
           <t>narrow mappings</t>
         </is>
       </c>
-      <c r="CY1" t="inlineStr">
+      <c r="DB1" t="inlineStr">
         <is>
           <t>broad mappings</t>
         </is>
       </c>
-      <c r="CZ1" t="inlineStr">
+      <c r="DC1" t="inlineStr">
         <is>
           <t>created_by</t>
         </is>
       </c>
-      <c r="DA1" t="inlineStr">
+      <c r="DD1" t="inlineStr">
         <is>
           <t>contributors</t>
         </is>
       </c>
-      <c r="DB1" t="inlineStr">
+      <c r="DE1" t="inlineStr">
         <is>
           <t>created_on</t>
         </is>
       </c>
-      <c r="DC1" t="inlineStr">
+      <c r="DF1" t="inlineStr">
         <is>
           <t>last_updated_on</t>
         </is>
       </c>
-      <c r="DD1" t="inlineStr">
+      <c r="DG1" t="inlineStr">
         <is>
           <t>modified_by</t>
         </is>
       </c>
-      <c r="DE1" t="inlineStr">
+      <c r="DH1" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
-      <c r="DF1" t="inlineStr">
+      <c r="DI1" t="inlineStr">
         <is>
           <t>rank</t>
         </is>
       </c>
-      <c r="DG1" t="inlineStr">
+      <c r="DJ1" t="inlineStr">
         <is>
           <t>categories</t>
         </is>
       </c>
-      <c r="DH1" t="inlineStr">
+      <c r="DK1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
@@ -1860,10 +1883,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation sqref="AE2:AE1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="AF2:AF1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"SUBJECT,OBJECT,PREDICATE,NODE,OTHER_ROLE"</formula1>
     </dataValidation>
-    <dataValidation sqref="AY2:AY1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="AZ2:AZ1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"UNCOMMITTED,PRESENT,ABSENT"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2103,7 +2126,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BQ1"/>
+  <dimension ref="A1:BR1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2259,200 +2282,205 @@
       </c>
       <c r="AD1" t="inlineStr">
         <is>
+          <t>id_prefixes_are_closed</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
           <t>definition_uri</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>local_names</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>conforms_to</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>implements</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>instantiates</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>extensions</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>annotations</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>alt_descriptions</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>deprecated</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>todos</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>comments</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>examples</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>in_subset</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>from_schema</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>imported_from</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>source</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>in_language</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>deprecated element has exact replacement</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>deprecated element has possible replacement</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>aliases</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>structured_aliases</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>mappings</t>
         </is>
       </c>
-      <c r="BD1" t="inlineStr">
+      <c r="BE1" t="inlineStr">
         <is>
           <t>exact mappings</t>
         </is>
       </c>
-      <c r="BE1" t="inlineStr">
+      <c r="BF1" t="inlineStr">
         <is>
           <t>close mappings</t>
         </is>
       </c>
-      <c r="BF1" t="inlineStr">
+      <c r="BG1" t="inlineStr">
         <is>
           <t>related mappings</t>
         </is>
       </c>
-      <c r="BG1" t="inlineStr">
+      <c r="BH1" t="inlineStr">
         <is>
           <t>narrow mappings</t>
         </is>
       </c>
-      <c r="BH1" t="inlineStr">
+      <c r="BI1" t="inlineStr">
         <is>
           <t>broad mappings</t>
         </is>
       </c>
-      <c r="BI1" t="inlineStr">
+      <c r="BJ1" t="inlineStr">
         <is>
           <t>created_by</t>
         </is>
       </c>
-      <c r="BJ1" t="inlineStr">
+      <c r="BK1" t="inlineStr">
         <is>
           <t>contributors</t>
         </is>
       </c>
-      <c r="BK1" t="inlineStr">
+      <c r="BL1" t="inlineStr">
         <is>
           <t>created_on</t>
         </is>
       </c>
-      <c r="BL1" t="inlineStr">
+      <c r="BM1" t="inlineStr">
         <is>
           <t>last_updated_on</t>
         </is>
       </c>
-      <c r="BM1" t="inlineStr">
+      <c r="BN1" t="inlineStr">
         <is>
           <t>modified_by</t>
         </is>
       </c>
-      <c r="BN1" t="inlineStr">
+      <c r="BO1" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
-      <c r="BO1" t="inlineStr">
+      <c r="BP1" t="inlineStr">
         <is>
           <t>rank</t>
         </is>
       </c>
-      <c r="BP1" t="inlineStr">
+      <c r="BQ1" t="inlineStr">
         <is>
           <t>categories</t>
         </is>
       </c>
-      <c r="BQ1" t="inlineStr">
+      <c r="BR1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
@@ -2695,7 +2723,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AL1"/>
+  <dimension ref="A1:AN1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2706,190 +2734,200 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>syntax</t>
+          <t>exact_number_dimensions</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>interpolated</t>
+          <t>minimum_number_dimensions</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>partial_match</t>
+          <t>maximum_number_dimensions</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>has_extra_dimensions</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>dimensions</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>extensions</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>annotations</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>alt_descriptions</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>deprecated</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>todos</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>comments</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>examples</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>in_subset</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>from_schema</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>imported_from</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>source</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>in_language</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>deprecated element has exact replacement</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>deprecated element has possible replacement</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>aliases</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>structured_aliases</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>mappings</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>exact mappings</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>close mappings</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>related mappings</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>narrow mappings</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>broad mappings</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>created_by</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>contributors</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>created_on</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>last_updated_on</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>modified_by</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>rank</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>categories</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
@@ -2901,6 +2939,563 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AM1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>alias</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>maximum_cardinality</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>minimum_cardinality</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>exact_cardinality</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>extensions</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>annotations</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>alt_descriptions</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>deprecated</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>todos</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>notes</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>examples</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>in_subset</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>from_schema</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>imported_from</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>in_language</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>see_also</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>deprecated element has exact replacement</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>deprecated element has possible replacement</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>aliases</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>structured_aliases</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>mappings</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>exact mappings</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>close mappings</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>related mappings</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>narrow mappings</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>broad mappings</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>created_by</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>contributors</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>created_on</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>last_updated_on</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>modified_by</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>categories</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>keywords</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:BL1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>version</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>imports</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>license</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>prefixes</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>emit_prefixes</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>default_curi_maps</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>default_prefix</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>default_range</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>subsets</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>types</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>enums</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>slot_definitions</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>classes</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>metamodel_version</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>source_file</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>source_file_date</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>source_file_size</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>generation_date</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>slot_names_unique</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>settings</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>id_prefixes</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>id_prefixes_are_closed</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>definition_uri</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>local_names</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>conforms_to</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>implements</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>instantiates</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>extensions</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>annotations</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>alt_descriptions</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>deprecated</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>todos</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>notes</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>examples</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>in_subset</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>from_schema</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>imported_from</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>in_language</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>see_also</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>deprecated element has exact replacement</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
+          <t>deprecated element has possible replacement</t>
+        </is>
+      </c>
+      <c r="AV1" t="inlineStr">
+        <is>
+          <t>aliases</t>
+        </is>
+      </c>
+      <c r="AW1" t="inlineStr">
+        <is>
+          <t>structured_aliases</t>
+        </is>
+      </c>
+      <c r="AX1" t="inlineStr">
+        <is>
+          <t>mappings</t>
+        </is>
+      </c>
+      <c r="AY1" t="inlineStr">
+        <is>
+          <t>exact mappings</t>
+        </is>
+      </c>
+      <c r="AZ1" t="inlineStr">
+        <is>
+          <t>close mappings</t>
+        </is>
+      </c>
+      <c r="BA1" t="inlineStr">
+        <is>
+          <t>related mappings</t>
+        </is>
+      </c>
+      <c r="BB1" t="inlineStr">
+        <is>
+          <t>narrow mappings</t>
+        </is>
+      </c>
+      <c r="BC1" t="inlineStr">
+        <is>
+          <t>broad mappings</t>
+        </is>
+      </c>
+      <c r="BD1" t="inlineStr">
+        <is>
+          <t>created_by</t>
+        </is>
+      </c>
+      <c r="BE1" t="inlineStr">
+        <is>
+          <t>contributors</t>
+        </is>
+      </c>
+      <c r="BF1" t="inlineStr">
+        <is>
+          <t>created_on</t>
+        </is>
+      </c>
+      <c r="BG1" t="inlineStr">
+        <is>
+          <t>last_updated_on</t>
+        </is>
+      </c>
+      <c r="BH1" t="inlineStr">
+        <is>
+          <t>modified_by</t>
+        </is>
+      </c>
+      <c r="BI1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="BJ1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="BK1" t="inlineStr">
+        <is>
+          <t>categories</t>
+        </is>
+      </c>
+      <c r="BL1" t="inlineStr">
+        <is>
+          <t>keywords</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2917,17 +3512,17 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>import_from</t>
+          <t>syntax</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>import_as</t>
+          <t>interpolated</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>import_map</t>
+          <t>partial_match</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -3103,373 +3698,6 @@
       <c r="AL1" t="inlineStr">
         <is>
           <t>keywords</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:BK1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>version</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>imports</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>license</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>prefixes</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>emit_prefixes</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>default_curi_maps</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>default_prefix</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>default_range</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>subsets</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>types</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>enums</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>slot_definitions</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>classes</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>metamodel_version</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>source_file</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>source_file_date</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>source_file_size</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>generation_date</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>slot_names_unique</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>settings</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>id_prefixes</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>definition_uri</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>local_names</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>conforms_to</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>implements</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>instantiates</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>extensions</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>annotations</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>alt_descriptions</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>deprecated</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>todos</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>notes</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>comments</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>examples</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>in_subset</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>from_schema</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>imported_from</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>source</t>
-        </is>
-      </c>
-      <c r="AQ1" t="inlineStr">
-        <is>
-          <t>in_language</t>
-        </is>
-      </c>
-      <c r="AR1" t="inlineStr">
-        <is>
-          <t>see_also</t>
-        </is>
-      </c>
-      <c r="AS1" t="inlineStr">
-        <is>
-          <t>deprecated element has exact replacement</t>
-        </is>
-      </c>
-      <c r="AT1" t="inlineStr">
-        <is>
-          <t>deprecated element has possible replacement</t>
-        </is>
-      </c>
-      <c r="AU1" t="inlineStr">
-        <is>
-          <t>aliases</t>
-        </is>
-      </c>
-      <c r="AV1" t="inlineStr">
-        <is>
-          <t>structured_aliases</t>
-        </is>
-      </c>
-      <c r="AW1" t="inlineStr">
-        <is>
-          <t>mappings</t>
-        </is>
-      </c>
-      <c r="AX1" t="inlineStr">
-        <is>
-          <t>exact mappings</t>
-        </is>
-      </c>
-      <c r="AY1" t="inlineStr">
-        <is>
-          <t>close mappings</t>
-        </is>
-      </c>
-      <c r="AZ1" t="inlineStr">
-        <is>
-          <t>related mappings</t>
-        </is>
-      </c>
-      <c r="BA1" t="inlineStr">
-        <is>
-          <t>narrow mappings</t>
-        </is>
-      </c>
-      <c r="BB1" t="inlineStr">
-        <is>
-          <t>broad mappings</t>
-        </is>
-      </c>
-      <c r="BC1" t="inlineStr">
-        <is>
-          <t>created_by</t>
-        </is>
-      </c>
-      <c r="BD1" t="inlineStr">
-        <is>
-          <t>contributors</t>
-        </is>
-      </c>
-      <c r="BE1" t="inlineStr">
-        <is>
-          <t>created_on</t>
-        </is>
-      </c>
-      <c r="BF1" t="inlineStr">
-        <is>
-          <t>last_updated_on</t>
-        </is>
-      </c>
-      <c r="BG1" t="inlineStr">
-        <is>
-          <t>modified_by</t>
-        </is>
-      </c>
-      <c r="BH1" t="inlineStr">
-        <is>
-          <t>status</t>
-        </is>
-      </c>
-      <c r="BI1" t="inlineStr">
-        <is>
-          <t>rank</t>
-        </is>
-      </c>
-      <c r="BJ1" t="inlineStr">
-        <is>
-          <t>categories</t>
-        </is>
-      </c>
-      <c r="BK1" t="inlineStr">
-        <is>
-          <t>keywords</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>setting_key</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>setting_value</t>
         </is>
       </c>
     </row>
@@ -3484,7 +3712,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:AL1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3495,12 +3723,192 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>prefix_prefix</t>
+          <t>import_from</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>prefix_reference</t>
+          <t>import_as</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>import_map</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>extensions</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>annotations</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>alt_descriptions</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>deprecated</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>todos</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>notes</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>examples</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>in_subset</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>from_schema</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>imported_from</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>in_language</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>see_also</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>deprecated element has exact replacement</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>deprecated element has possible replacement</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>aliases</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>structured_aliases</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>mappings</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>exact mappings</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>close mappings</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>related mappings</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>narrow mappings</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>broad mappings</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>created_by</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>contributors</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>created_on</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>last_updated_on</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>modified_by</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>categories</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>keywords</t>
         </is>
       </c>
     </row>
@@ -3526,12 +3934,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>local_name_source</t>
+          <t>setting_key</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>local_name_value</t>
+          <t>setting_value</t>
         </is>
       </c>
     </row>
@@ -3546,7 +3954,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3557,17 +3965,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>value</t>
+          <t>prefix_prefix</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>value_description</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>value_object</t>
+          <t>prefix_reference</t>
         </is>
       </c>
     </row>
@@ -3593,12 +3996,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>alt_description_source</t>
+          <t>local_name_source</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>alt_description_text</t>
+          <t>local_name_value</t>
         </is>
       </c>
     </row>
@@ -3608,6 +4011,73 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>value_description</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>value_object</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>alt_description_source</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>alt_description_text</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3818,7 +4288,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4029,7 +4499,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4082,83 +4552,6 @@
       <c r="H1" t="inlineStr">
         <is>
           <t>iec61360code</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>annotations</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>extension_tag</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>extension_value</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>extensions</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>extension_tag</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>extension_value</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>extensions</t>
         </is>
       </c>
     </row>
@@ -4253,13 +4646,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BH1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4270,6 +4663,101 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>annotations</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>extension_tag</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>extension_value</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>extensions</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>extension_tag</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>extension_value</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>extensions</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:BI1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>typeof</t>
         </is>
       </c>
@@ -4370,200 +4858,205 @@
       </c>
       <c r="U1" t="inlineStr">
         <is>
+          <t>id_prefixes_are_closed</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
           <t>definition_uri</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>local_names</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>conforms_to</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>implements</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>instantiates</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>extensions</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>annotations</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>alt_descriptions</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>deprecated</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>todos</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>comments</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>examples</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>in_subset</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>from_schema</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>imported_from</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>source</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>in_language</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>deprecated element has exact replacement</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>deprecated element has possible replacement</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>aliases</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>structured_aliases</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>mappings</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>exact mappings</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>close mappings</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>related mappings</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>narrow mappings</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>broad mappings</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>created_by</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>contributors</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>created_on</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>last_updated_on</t>
         </is>
       </c>
-      <c r="BD1" t="inlineStr">
+      <c r="BE1" t="inlineStr">
         <is>
           <t>modified_by</t>
         </is>
       </c>
-      <c r="BE1" t="inlineStr">
+      <c r="BF1" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
-      <c r="BF1" t="inlineStr">
+      <c r="BG1" t="inlineStr">
         <is>
           <t>rank</t>
         </is>
       </c>
-      <c r="BG1" t="inlineStr">
+      <c r="BH1" t="inlineStr">
         <is>
           <t>categories</t>
         </is>
       </c>
-      <c r="BH1" t="inlineStr">
+      <c r="BI1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
@@ -4580,7 +5073,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AP1"/>
+  <dimension ref="A1:AQ1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4601,200 +5094,205 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>id_prefixes_are_closed</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>definition_uri</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>local_names</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>conforms_to</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>implements</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>instantiates</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>extensions</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>annotations</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>alt_descriptions</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>deprecated</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>todos</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>comments</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>examples</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>in_subset</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>from_schema</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>imported_from</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>source</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>in_language</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>deprecated element has exact replacement</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>deprecated element has possible replacement</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>aliases</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>structured_aliases</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>mappings</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>exact mappings</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>close mappings</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>related mappings</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>narrow mappings</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>broad mappings</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>created_by</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>contributors</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>created_on</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>last_updated_on</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>modified_by</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>rank</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>categories</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
@@ -4879,7 +5377,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"CODE,CURIE,URI,FHIR_CODING"</formula1>
+      <formula1>"CODE,CURIE,URI,FHIR_CODING,LABEL"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4960,7 +5458,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"CODE,CURIE,URI,FHIR_CODING"</formula1>
+      <formula1>"CODE,CURIE,URI,FHIR_CODING,LABEL"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4973,7 +5471,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BI1"/>
+  <dimension ref="A1:BJ1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5089,200 +5587,205 @@
       </c>
       <c r="V1" t="inlineStr">
         <is>
+          <t>id_prefixes_are_closed</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
           <t>definition_uri</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>local_names</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>conforms_to</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>implements</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>instantiates</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>extensions</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>annotations</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>alt_descriptions</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>deprecated</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>todos</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>comments</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>examples</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>in_subset</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>from_schema</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>imported_from</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>source</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>in_language</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>deprecated element has exact replacement</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>deprecated element has possible replacement</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>aliases</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>structured_aliases</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>mappings</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>exact mappings</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>close mappings</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>related mappings</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>narrow mappings</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>broad mappings</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>created_by</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>contributors</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>created_on</t>
         </is>
       </c>
-      <c r="BD1" t="inlineStr">
+      <c r="BE1" t="inlineStr">
         <is>
           <t>last_updated_on</t>
         </is>
       </c>
-      <c r="BE1" t="inlineStr">
+      <c r="BF1" t="inlineStr">
         <is>
           <t>modified_by</t>
         </is>
       </c>
-      <c r="BF1" t="inlineStr">
+      <c r="BG1" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
-      <c r="BG1" t="inlineStr">
+      <c r="BH1" t="inlineStr">
         <is>
           <t>rank</t>
         </is>
       </c>
-      <c r="BH1" t="inlineStr">
+      <c r="BI1" t="inlineStr">
         <is>
           <t>categories</t>
         </is>
       </c>
-      <c r="BI1" t="inlineStr">
+      <c r="BJ1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
@@ -5291,7 +5794,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"CODE,CURIE,URI,FHIR_CODING"</formula1>
+      <formula1>"CODE,CURIE,URI,FHIR_CODING,LABEL"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add Linked Open Vocabularies recommended ontology metadata
Signed-off-by: Vincent Kelleher <vincent.kelleher@gaia-x.eu>
</commit_message>
<xml_diff>
--- a/linkml_model/excel/meta.xlsx
+++ b/linkml_model/excel/meta.xlsx
@@ -15,30 +15,33 @@
     <sheet name="enum_expression" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="anonymous_enum_expression" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="enum_definition" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="match_query" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="reachability_query" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="structured_alias" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="path_expression" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="anonymous_slot_expression" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="slot_definition" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="anonymous_class_expression" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="class_definition" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="class_rule" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="array_expression" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="dimension_expression" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="pattern_expression" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="import_expression" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="setting" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="prefix" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="local_name" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="example" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="alt_description" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="permissible_value" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="unique_key" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="UnitOfMeasure" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="annotation" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet name="AnyValue" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet name="extension" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="enum_binding" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="match_query" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="reachability_query" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="structured_alias" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="path_expression" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="anonymous_slot_expression" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="slot_definition" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="anonymous_class_expression" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="class_definition" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="class_rule" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="array_expression" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="dimension_expression" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="pattern_expression" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="import_expression" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="setting" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="prefix" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="local_name" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="example" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="alt_description" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="permissible_value" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="unique_key" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="type_mapping" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="extra_slots_expression" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="UnitOfMeasure" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="annotation" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="AnyValue" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="extension" sheetId="35" state="visible" r:id="rId35"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -462,7 +465,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,32 +476,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>identifier_pattern</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>source_ontology</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>source_nodes</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>relationship_types</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>is_direct</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>include_self</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>traverse_up</t>
         </is>
       </c>
     </row>
@@ -513,7 +496,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AK1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -524,6 +507,57 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>source_ontology</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>source_nodes</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>relationship_types</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>is_direct</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>include_self</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>traverse_up</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AL1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>literal_form</t>
         </is>
       </c>
@@ -539,170 +573,175 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>alias_contexts</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>extensions</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>annotations</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>alt_descriptions</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>deprecated</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>todos</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>comments</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>examples</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>in_subset</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>from_schema</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>imported_from</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>source</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>in_language</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>deprecated element has exact replacement</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>deprecated element has possible replacement</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>aliases</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>structured_aliases</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>mappings</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>exact mappings</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>close mappings</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>related mappings</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>narrow mappings</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>broad mappings</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>created_by</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>contributors</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>created_on</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>last_updated_on</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>modified_by</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>rank</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
@@ -718,7 +757,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -954,13 +993,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BJ1"/>
+  <dimension ref="A1:BM1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -986,295 +1025,310 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>bindings</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>required</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>recommended</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>multivalued</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
         <is>
           <t>inlined</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>inlined_as_list</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>minimum_value</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>maximum_value</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>pattern</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>structured_pattern</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>unit</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>implicit_prefix</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>value_presence</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>equals_string</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>equals_string_in</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>equals_number</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>equals_expression</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>exact_cardinality</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>minimum_cardinality</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>maximum_cardinality</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>has_member</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>all_members</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>none_of</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>exactly_one_of</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>any_of</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>all_of</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>array</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
         <is>
           <t>extensions</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>annotations</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>alt_descriptions</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>deprecated</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>todos</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>comments</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>examples</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>in_subset</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>from_schema</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>imported_from</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>source</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>in_language</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>deprecated element has exact replacement</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>deprecated element has possible replacement</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>aliases</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>structured_aliases</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>mappings</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>exact mappings</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>close mappings</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>related mappings</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>narrow mappings</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>broad mappings</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BE1" t="inlineStr">
         <is>
           <t>created_by</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BF1" t="inlineStr">
         <is>
           <t>contributors</t>
         </is>
       </c>
-      <c r="BD1" t="inlineStr">
+      <c r="BG1" t="inlineStr">
         <is>
           <t>created_on</t>
         </is>
       </c>
-      <c r="BE1" t="inlineStr">
+      <c r="BH1" t="inlineStr">
         <is>
           <t>last_updated_on</t>
         </is>
       </c>
-      <c r="BF1" t="inlineStr">
+      <c r="BI1" t="inlineStr">
         <is>
           <t>modified_by</t>
         </is>
       </c>
-      <c r="BG1" t="inlineStr">
+      <c r="BJ1" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
-      <c r="BH1" t="inlineStr">
+      <c r="BK1" t="inlineStr">
         <is>
           <t>rank</t>
         </is>
       </c>
-      <c r="BI1" t="inlineStr">
+      <c r="BL1" t="inlineStr">
         <is>
           <t>categories</t>
         </is>
       </c>
-      <c r="BJ1" t="inlineStr">
+      <c r="BM1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
@@ -1282,7 +1336,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation sqref="N2:N1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="P2:P1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"UNCOMMITTED,PRESENT,ABSENT"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1290,13 +1344,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DK1"/>
+  <dimension ref="A1:DM1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1322,560 +1376,570 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>inherited</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>readonly</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>ifabsent</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>list_elements_unique</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>list_elements_ordered</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>shared</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>key</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>identifier</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>designates_type</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>alias</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>owner</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>domain_of</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>subproperty_of</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>symmetric</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>reflexive</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>locally_reflexive</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>irreflexive</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>asymmetric</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>transitive</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>inverse</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>is_class_field</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>transitive_form_of</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>reflexive_transitive_form_of</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>role</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>is_usage_slot</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>usage_slot_name</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>relational_role</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>slot_group</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>is_grouping_slot</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>path_rule</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>disjoint_with</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>children_are_mutually_disjoint</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>union_of</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>type_mappings</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>range</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>range_expression</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>enum_range</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>bindings</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>required</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>recommended</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
           <t>multivalued</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>inlined</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>inlined_as_list</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
+          <t>minimum_value</t>
+        </is>
+      </c>
+      <c r="AV1" t="inlineStr">
+        <is>
+          <t>maximum_value</t>
+        </is>
+      </c>
+      <c r="AW1" t="inlineStr">
+        <is>
+          <t>pattern</t>
+        </is>
+      </c>
+      <c r="AX1" t="inlineStr">
+        <is>
+          <t>structured_pattern</t>
+        </is>
+      </c>
+      <c r="AY1" t="inlineStr">
+        <is>
+          <t>unit</t>
+        </is>
+      </c>
+      <c r="AZ1" t="inlineStr">
+        <is>
+          <t>implicit_prefix</t>
+        </is>
+      </c>
+      <c r="BA1" t="inlineStr">
+        <is>
+          <t>value_presence</t>
+        </is>
+      </c>
+      <c r="BB1" t="inlineStr">
+        <is>
+          <t>equals_string</t>
+        </is>
+      </c>
+      <c r="BC1" t="inlineStr">
+        <is>
+          <t>equals_string_in</t>
+        </is>
+      </c>
+      <c r="BD1" t="inlineStr">
+        <is>
+          <t>equals_number</t>
+        </is>
+      </c>
+      <c r="BE1" t="inlineStr">
+        <is>
+          <t>equals_expression</t>
+        </is>
+      </c>
+      <c r="BF1" t="inlineStr">
+        <is>
+          <t>exact_cardinality</t>
+        </is>
+      </c>
+      <c r="BG1" t="inlineStr">
+        <is>
+          <t>minimum_cardinality</t>
+        </is>
+      </c>
+      <c r="BH1" t="inlineStr">
+        <is>
+          <t>maximum_cardinality</t>
+        </is>
+      </c>
+      <c r="BI1" t="inlineStr">
+        <is>
+          <t>has_member</t>
+        </is>
+      </c>
+      <c r="BJ1" t="inlineStr">
+        <is>
+          <t>all_members</t>
+        </is>
+      </c>
+      <c r="BK1" t="inlineStr">
+        <is>
+          <t>none_of</t>
+        </is>
+      </c>
+      <c r="BL1" t="inlineStr">
+        <is>
+          <t>exactly_one_of</t>
+        </is>
+      </c>
+      <c r="BM1" t="inlineStr">
+        <is>
+          <t>any_of</t>
+        </is>
+      </c>
+      <c r="BN1" t="inlineStr">
+        <is>
+          <t>all_of</t>
+        </is>
+      </c>
+      <c r="BO1" t="inlineStr">
         <is>
           <t>array</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>inherited</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>readonly</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>ifabsent</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>list_elements_unique</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>list_elements_ordered</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>shared</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>key</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>identifier</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>designates_type</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>alias</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>owner</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>domain_of</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>subproperty_of</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>symmetric</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>reflexive</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>locally_reflexive</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>irreflexive</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>asymmetric</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>transitive</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>inverse</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>is_class_field</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>transitive_form_of</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>reflexive_transitive_form_of</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>role</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>is_usage_slot</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>usage_slot_name</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>relational_role</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>slot_group</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>is_grouping_slot</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>path_rule</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>disjoint_with</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>children_are_mutually_disjoint</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>union_of</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>range</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>range_expression</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>enum_range</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>required</t>
-        </is>
-      </c>
-      <c r="AQ1" t="inlineStr">
-        <is>
-          <t>recommended</t>
-        </is>
-      </c>
-      <c r="AR1" t="inlineStr">
-        <is>
-          <t>inlined</t>
-        </is>
-      </c>
-      <c r="AS1" t="inlineStr">
-        <is>
-          <t>inlined_as_list</t>
-        </is>
-      </c>
-      <c r="AT1" t="inlineStr">
-        <is>
-          <t>minimum_value</t>
-        </is>
-      </c>
-      <c r="AU1" t="inlineStr">
-        <is>
-          <t>maximum_value</t>
-        </is>
-      </c>
-      <c r="AV1" t="inlineStr">
-        <is>
-          <t>pattern</t>
-        </is>
-      </c>
-      <c r="AW1" t="inlineStr">
-        <is>
-          <t>structured_pattern</t>
-        </is>
-      </c>
-      <c r="AX1" t="inlineStr">
-        <is>
-          <t>unit</t>
-        </is>
-      </c>
-      <c r="AY1" t="inlineStr">
-        <is>
-          <t>implicit_prefix</t>
-        </is>
-      </c>
-      <c r="AZ1" t="inlineStr">
-        <is>
-          <t>value_presence</t>
-        </is>
-      </c>
-      <c r="BA1" t="inlineStr">
-        <is>
-          <t>equals_string</t>
-        </is>
-      </c>
-      <c r="BB1" t="inlineStr">
-        <is>
-          <t>equals_string_in</t>
-        </is>
-      </c>
-      <c r="BC1" t="inlineStr">
-        <is>
-          <t>equals_number</t>
-        </is>
-      </c>
-      <c r="BD1" t="inlineStr">
-        <is>
-          <t>equals_expression</t>
-        </is>
-      </c>
-      <c r="BE1" t="inlineStr">
-        <is>
-          <t>exact_cardinality</t>
-        </is>
-      </c>
-      <c r="BF1" t="inlineStr">
-        <is>
-          <t>minimum_cardinality</t>
-        </is>
-      </c>
-      <c r="BG1" t="inlineStr">
-        <is>
-          <t>maximum_cardinality</t>
-        </is>
-      </c>
-      <c r="BH1" t="inlineStr">
-        <is>
-          <t>has_member</t>
-        </is>
-      </c>
-      <c r="BI1" t="inlineStr">
-        <is>
-          <t>all_members</t>
-        </is>
-      </c>
-      <c r="BJ1" t="inlineStr">
-        <is>
-          <t>none_of</t>
-        </is>
-      </c>
-      <c r="BK1" t="inlineStr">
-        <is>
-          <t>exactly_one_of</t>
-        </is>
-      </c>
-      <c r="BL1" t="inlineStr">
-        <is>
-          <t>any_of</t>
-        </is>
-      </c>
-      <c r="BM1" t="inlineStr">
-        <is>
-          <t>all_of</t>
-        </is>
-      </c>
-      <c r="BN1" t="inlineStr">
+      <c r="BP1" t="inlineStr">
         <is>
           <t>is_a</t>
         </is>
       </c>
-      <c r="BO1" t="inlineStr">
+      <c r="BQ1" t="inlineStr">
         <is>
           <t>abstract</t>
         </is>
       </c>
-      <c r="BP1" t="inlineStr">
+      <c r="BR1" t="inlineStr">
         <is>
           <t>mixin</t>
         </is>
       </c>
-      <c r="BQ1" t="inlineStr">
+      <c r="BS1" t="inlineStr">
         <is>
           <t>mixins</t>
         </is>
       </c>
-      <c r="BR1" t="inlineStr">
+      <c r="BT1" t="inlineStr">
         <is>
           <t>apply_to</t>
         </is>
       </c>
-      <c r="BS1" t="inlineStr">
+      <c r="BU1" t="inlineStr">
         <is>
           <t>values_from</t>
         </is>
       </c>
-      <c r="BT1" t="inlineStr">
+      <c r="BV1" t="inlineStr">
         <is>
           <t>string_serialization</t>
         </is>
       </c>
-      <c r="BU1" t="inlineStr">
+      <c r="BW1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="BV1" t="inlineStr">
+      <c r="BX1" t="inlineStr">
         <is>
           <t>id_prefixes</t>
         </is>
       </c>
-      <c r="BW1" t="inlineStr">
+      <c r="BY1" t="inlineStr">
         <is>
           <t>id_prefixes_are_closed</t>
         </is>
       </c>
-      <c r="BX1" t="inlineStr">
+      <c r="BZ1" t="inlineStr">
         <is>
           <t>definition_uri</t>
         </is>
       </c>
-      <c r="BY1" t="inlineStr">
+      <c r="CA1" t="inlineStr">
         <is>
           <t>local_names</t>
         </is>
       </c>
-      <c r="BZ1" t="inlineStr">
+      <c r="CB1" t="inlineStr">
         <is>
           <t>conforms_to</t>
         </is>
       </c>
-      <c r="CA1" t="inlineStr">
+      <c r="CC1" t="inlineStr">
         <is>
           <t>implements</t>
         </is>
       </c>
-      <c r="CB1" t="inlineStr">
+      <c r="CD1" t="inlineStr">
         <is>
           <t>instantiates</t>
         </is>
       </c>
-      <c r="CC1" t="inlineStr">
+      <c r="CE1" t="inlineStr">
         <is>
           <t>extensions</t>
         </is>
       </c>
-      <c r="CD1" t="inlineStr">
+      <c r="CF1" t="inlineStr">
         <is>
           <t>annotations</t>
         </is>
       </c>
-      <c r="CE1" t="inlineStr">
+      <c r="CG1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="CF1" t="inlineStr">
+      <c r="CH1" t="inlineStr">
         <is>
           <t>alt_descriptions</t>
         </is>
       </c>
-      <c r="CG1" t="inlineStr">
+      <c r="CI1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="CH1" t="inlineStr">
+      <c r="CJ1" t="inlineStr">
         <is>
           <t>deprecated</t>
         </is>
       </c>
-      <c r="CI1" t="inlineStr">
+      <c r="CK1" t="inlineStr">
         <is>
           <t>todos</t>
         </is>
       </c>
-      <c r="CJ1" t="inlineStr">
+      <c r="CL1" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
       </c>
-      <c r="CK1" t="inlineStr">
+      <c r="CM1" t="inlineStr">
         <is>
           <t>comments</t>
         </is>
       </c>
-      <c r="CL1" t="inlineStr">
+      <c r="CN1" t="inlineStr">
         <is>
           <t>examples</t>
         </is>
       </c>
-      <c r="CM1" t="inlineStr">
+      <c r="CO1" t="inlineStr">
         <is>
           <t>in_subset</t>
         </is>
       </c>
-      <c r="CN1" t="inlineStr">
+      <c r="CP1" t="inlineStr">
         <is>
           <t>from_schema</t>
         </is>
       </c>
-      <c r="CO1" t="inlineStr">
+      <c r="CQ1" t="inlineStr">
         <is>
           <t>imported_from</t>
         </is>
       </c>
-      <c r="CP1" t="inlineStr">
+      <c r="CR1" t="inlineStr">
         <is>
           <t>source</t>
         </is>
       </c>
-      <c r="CQ1" t="inlineStr">
+      <c r="CS1" t="inlineStr">
         <is>
           <t>in_language</t>
         </is>
       </c>
-      <c r="CR1" t="inlineStr">
+      <c r="CT1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="CS1" t="inlineStr">
+      <c r="CU1" t="inlineStr">
         <is>
           <t>deprecated element has exact replacement</t>
         </is>
       </c>
-      <c r="CT1" t="inlineStr">
+      <c r="CV1" t="inlineStr">
         <is>
           <t>deprecated element has possible replacement</t>
         </is>
       </c>
-      <c r="CU1" t="inlineStr">
+      <c r="CW1" t="inlineStr">
         <is>
           <t>aliases</t>
         </is>
       </c>
-      <c r="CV1" t="inlineStr">
+      <c r="CX1" t="inlineStr">
         <is>
           <t>structured_aliases</t>
         </is>
       </c>
-      <c r="CW1" t="inlineStr">
+      <c r="CY1" t="inlineStr">
         <is>
           <t>mappings</t>
         </is>
       </c>
-      <c r="CX1" t="inlineStr">
+      <c r="CZ1" t="inlineStr">
         <is>
           <t>exact mappings</t>
         </is>
       </c>
-      <c r="CY1" t="inlineStr">
+      <c r="DA1" t="inlineStr">
         <is>
           <t>close mappings</t>
         </is>
       </c>
-      <c r="CZ1" t="inlineStr">
+      <c r="DB1" t="inlineStr">
         <is>
           <t>related mappings</t>
         </is>
       </c>
-      <c r="DA1" t="inlineStr">
+      <c r="DC1" t="inlineStr">
         <is>
           <t>narrow mappings</t>
         </is>
       </c>
-      <c r="DB1" t="inlineStr">
+      <c r="DD1" t="inlineStr">
         <is>
           <t>broad mappings</t>
         </is>
       </c>
-      <c r="DC1" t="inlineStr">
+      <c r="DE1" t="inlineStr">
         <is>
           <t>created_by</t>
         </is>
       </c>
-      <c r="DD1" t="inlineStr">
+      <c r="DF1" t="inlineStr">
         <is>
           <t>contributors</t>
         </is>
       </c>
-      <c r="DE1" t="inlineStr">
+      <c r="DG1" t="inlineStr">
         <is>
           <t>created_on</t>
         </is>
       </c>
-      <c r="DF1" t="inlineStr">
+      <c r="DH1" t="inlineStr">
         <is>
           <t>last_updated_on</t>
         </is>
       </c>
-      <c r="DG1" t="inlineStr">
+      <c r="DI1" t="inlineStr">
         <is>
           <t>modified_by</t>
         </is>
       </c>
-      <c r="DH1" t="inlineStr">
+      <c r="DJ1" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
-      <c r="DI1" t="inlineStr">
+      <c r="DK1" t="inlineStr">
         <is>
           <t>rank</t>
         </is>
       </c>
-      <c r="DJ1" t="inlineStr">
+      <c r="DL1" t="inlineStr">
         <is>
           <t>categories</t>
         </is>
       </c>
-      <c r="DK1" t="inlineStr">
+      <c r="DM1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
@@ -1883,10 +1947,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation sqref="AF2:AF1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="AD2:AD1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"SUBJECT,OBJECT,PREDICATE,NODE,OTHER_ROLE"</formula1>
     </dataValidation>
-    <dataValidation sqref="AZ2:AZ1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="BA2:BA1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"UNCOMMITTED,PRESENT,ABSENT"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1894,7 +1958,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2120,13 +2184,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BR1"/>
+  <dimension ref="A1:BS1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2212,275 +2276,280 @@
       </c>
       <c r="P1" t="inlineStr">
         <is>
+          <t>extra_slots</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
           <t>any_of</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>exactly_one_of</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>none_of</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>all_of</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>slot_conditions</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>is_a</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>abstract</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>mixin</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>mixins</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>apply_to</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>values_from</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>string_serialization</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>id_prefixes</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>id_prefixes_are_closed</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>definition_uri</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>local_names</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>conforms_to</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>implements</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>instantiates</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>extensions</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>annotations</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>alt_descriptions</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>deprecated</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>todos</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>comments</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>examples</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>in_subset</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>from_schema</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>imported_from</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>source</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>in_language</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>deprecated element has exact replacement</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>deprecated element has possible replacement</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>aliases</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>structured_aliases</t>
         </is>
       </c>
-      <c r="BD1" t="inlineStr">
+      <c r="BE1" t="inlineStr">
         <is>
           <t>mappings</t>
         </is>
       </c>
-      <c r="BE1" t="inlineStr">
+      <c r="BF1" t="inlineStr">
         <is>
           <t>exact mappings</t>
         </is>
       </c>
-      <c r="BF1" t="inlineStr">
+      <c r="BG1" t="inlineStr">
         <is>
           <t>close mappings</t>
         </is>
       </c>
-      <c r="BG1" t="inlineStr">
+      <c r="BH1" t="inlineStr">
         <is>
           <t>related mappings</t>
         </is>
       </c>
-      <c r="BH1" t="inlineStr">
+      <c r="BI1" t="inlineStr">
         <is>
           <t>narrow mappings</t>
         </is>
       </c>
-      <c r="BI1" t="inlineStr">
+      <c r="BJ1" t="inlineStr">
         <is>
           <t>broad mappings</t>
         </is>
       </c>
-      <c r="BJ1" t="inlineStr">
+      <c r="BK1" t="inlineStr">
         <is>
           <t>created_by</t>
         </is>
       </c>
-      <c r="BK1" t="inlineStr">
+      <c r="BL1" t="inlineStr">
         <is>
           <t>contributors</t>
         </is>
       </c>
-      <c r="BL1" t="inlineStr">
+      <c r="BM1" t="inlineStr">
         <is>
           <t>created_on</t>
         </is>
       </c>
-      <c r="BM1" t="inlineStr">
+      <c r="BN1" t="inlineStr">
         <is>
           <t>last_updated_on</t>
         </is>
       </c>
-      <c r="BN1" t="inlineStr">
+      <c r="BO1" t="inlineStr">
         <is>
           <t>modified_by</t>
         </is>
       </c>
-      <c r="BO1" t="inlineStr">
+      <c r="BP1" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
-      <c r="BP1" t="inlineStr">
+      <c r="BQ1" t="inlineStr">
         <is>
           <t>rank</t>
         </is>
       </c>
-      <c r="BQ1" t="inlineStr">
+      <c r="BR1" t="inlineStr">
         <is>
           <t>categories</t>
         </is>
       </c>
-      <c r="BR1" t="inlineStr">
+      <c r="BS1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
@@ -2491,7 +2560,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2707,227 +2776,6 @@
         </is>
       </c>
       <c r="AO1" t="inlineStr">
-        <is>
-          <t>keywords</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AN1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>exact_number_dimensions</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>minimum_number_dimensions</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>maximum_number_dimensions</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>has_extra_dimensions</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>dimensions</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>extensions</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>annotations</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>alt_descriptions</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>deprecated</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>todos</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>notes</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>comments</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>examples</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>in_subset</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>from_schema</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>imported_from</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>source</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>in_language</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>see_also</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>deprecated element has exact replacement</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>deprecated element has possible replacement</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>aliases</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>structured_aliases</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>mappings</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>exact mappings</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>close mappings</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>related mappings</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>narrow mappings</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>broad mappings</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>created_by</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>contributors</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>created_on</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>last_updated_on</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>modified_by</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>status</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>rank</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>categories</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
@@ -2955,22 +2803,22 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>alias</t>
+          <t>exact_number_dimensions</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>maximum_cardinality</t>
+          <t>minimum_number_dimensions</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>minimum_cardinality</t>
+          <t>maximum_number_dimensions</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>exact_cardinality</t>
+          <t>dimensions</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
@@ -3160,7 +3008,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BL1"/>
+  <dimension ref="A1:BM1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3276,215 +3124,220 @@
       </c>
       <c r="V1" t="inlineStr">
         <is>
+          <t>bindings</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
           <t>name</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>id_prefixes</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>id_prefixes_are_closed</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>definition_uri</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>local_names</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>conforms_to</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>implements</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>instantiates</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>extensions</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>annotations</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>alt_descriptions</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>deprecated</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>todos</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>comments</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>examples</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>in_subset</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>from_schema</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>imported_from</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>source</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>in_language</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>deprecated element has exact replacement</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>deprecated element has possible replacement</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>aliases</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>structured_aliases</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>mappings</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>exact mappings</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>close mappings</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>related mappings</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>narrow mappings</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>broad mappings</t>
         </is>
       </c>
-      <c r="BD1" t="inlineStr">
+      <c r="BE1" t="inlineStr">
         <is>
           <t>created_by</t>
         </is>
       </c>
-      <c r="BE1" t="inlineStr">
+      <c r="BF1" t="inlineStr">
         <is>
           <t>contributors</t>
         </is>
       </c>
-      <c r="BF1" t="inlineStr">
+      <c r="BG1" t="inlineStr">
         <is>
           <t>created_on</t>
         </is>
       </c>
-      <c r="BG1" t="inlineStr">
+      <c r="BH1" t="inlineStr">
         <is>
           <t>last_updated_on</t>
         </is>
       </c>
-      <c r="BH1" t="inlineStr">
+      <c r="BI1" t="inlineStr">
         <is>
           <t>modified_by</t>
         </is>
       </c>
-      <c r="BI1" t="inlineStr">
+      <c r="BJ1" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
-      <c r="BJ1" t="inlineStr">
+      <c r="BK1" t="inlineStr">
         <is>
           <t>rank</t>
         </is>
       </c>
-      <c r="BK1" t="inlineStr">
+      <c r="BL1" t="inlineStr">
         <is>
           <t>categories</t>
         </is>
       </c>
-      <c r="BL1" t="inlineStr">
+      <c r="BM1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
@@ -3501,7 +3354,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AL1"/>
+  <dimension ref="A1:AM1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3512,190 +3365,195 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>syntax</t>
+          <t>alias</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>interpolated</t>
+          <t>maximum_cardinality</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>partial_match</t>
+          <t>minimum_cardinality</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>exact_cardinality</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>extensions</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>annotations</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>alt_descriptions</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>deprecated</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>todos</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>comments</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>examples</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>in_subset</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>from_schema</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>imported_from</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>source</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>in_language</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>deprecated element has exact replacement</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>deprecated element has possible replacement</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>aliases</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>structured_aliases</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>mappings</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>exact mappings</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>close mappings</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>related mappings</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>narrow mappings</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>broad mappings</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>created_by</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>contributors</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>created_on</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>last_updated_on</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>modified_by</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>rank</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>categories</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
@@ -3723,17 +3581,17 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>import_from</t>
+          <t>syntax</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>import_as</t>
+          <t>interpolated</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>import_map</t>
+          <t>partial_match</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -3923,7 +3781,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:AL1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3934,12 +3792,192 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>setting_key</t>
+          <t>import_from</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>setting_value</t>
+          <t>import_as</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>import_map</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>extensions</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>annotations</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>alt_descriptions</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>deprecated</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>todos</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>notes</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>examples</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>in_subset</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>from_schema</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>imported_from</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>in_language</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>see_also</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>deprecated element has exact replacement</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>deprecated element has possible replacement</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>aliases</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>structured_aliases</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>mappings</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>exact mappings</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>close mappings</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>related mappings</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>narrow mappings</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>broad mappings</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>created_by</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>contributors</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>created_on</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>last_updated_on</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>modified_by</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>categories</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>keywords</t>
         </is>
       </c>
     </row>
@@ -3965,12 +4003,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>prefix_prefix</t>
+          <t>setting_key</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>prefix_reference</t>
+          <t>setting_value</t>
         </is>
       </c>
     </row>
@@ -3996,12 +4034,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>local_name_source</t>
+          <t>prefix_prefix</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>local_name_value</t>
+          <t>prefix_reference</t>
         </is>
       </c>
     </row>
@@ -4011,6 +4049,37 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>local_name_source</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>local_name_value</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4046,7 +4115,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4077,7 +4146,238 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AP1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>meaning</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>unit</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>instantiates</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>implements</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>is_a</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>mixins</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>extensions</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>annotations</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>alt_descriptions</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>deprecated</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>todos</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>notes</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>examples</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>in_subset</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>from_schema</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>imported_from</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>in_language</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>see_also</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>deprecated element has exact replacement</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>deprecated element has possible replacement</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>aliases</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>structured_aliases</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>mappings</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>exact mappings</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>close mappings</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>related mappings</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>narrow mappings</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>broad mappings</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>created_by</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>contributors</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>created_on</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>last_updated_on</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>modified_by</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>categories</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>keywords</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4094,34 +4394,34 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>unique_key_name</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>unique_key_slots</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>consider_nulls_inequal</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>extensions</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>annotations</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>description</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>meaning</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>unit</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>extensions</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>annotations</t>
-        </is>
-      </c>
       <c r="G1" t="inlineStr">
         <is>
           <t>alt_descriptions</t>
@@ -4280,278 +4580,6 @@
       <c r="AL1" t="inlineStr">
         <is>
           <t>keywords</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AL1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>unique_key_name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>unique_key_slots</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>consider_nulls_inequal</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>extensions</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>annotations</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>alt_descriptions</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>deprecated</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>todos</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>notes</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>comments</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>examples</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>in_subset</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>from_schema</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>imported_from</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>source</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>in_language</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>see_also</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>deprecated element has exact replacement</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>deprecated element has possible replacement</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>aliases</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>structured_aliases</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>mappings</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>exact mappings</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>close mappings</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>related mappings</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>narrow mappings</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>broad mappings</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>created_by</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>contributors</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>created_on</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>last_updated_on</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>modified_by</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>status</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>rank</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>categories</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>keywords</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>symbol</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>abbreviation</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>descriptive_name</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>exact mappings</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>ucum_code</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>derivation</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>has_quantity_kind</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>iec61360code</t>
         </is>
       </c>
     </row>
@@ -4652,6 +4680,309 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:AL1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>framework_key</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>mapped_type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>string_serialization</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>extensions</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>annotations</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>alt_descriptions</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>deprecated</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>todos</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>notes</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>examples</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>in_subset</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>from_schema</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>imported_from</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>in_language</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>see_also</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>deprecated element has exact replacement</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>deprecated element has possible replacement</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>aliases</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>structured_aliases</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>mappings</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>exact mappings</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>close mappings</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>related mappings</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>narrow mappings</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>broad mappings</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>created_by</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>contributors</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>created_on</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>last_updated_on</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>modified_by</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>categories</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>keywords</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>allowed</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>range_expression</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>symbol</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>abbreviation</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>descriptive_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>exact mappings</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>ucum_code</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>derivation</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>has_quantity_kind</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>iec61360code</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4687,7 +5018,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4705,7 +5036,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -5807,7 +6138,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:AM1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5818,16 +6149,209 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>identifier_pattern</t>
+          <t>range</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>source_ontology</t>
+          <t>obligation_level</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>binds_value_of</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>pv_formula</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>extensions</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>annotations</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>alt_descriptions</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>deprecated</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>todos</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>notes</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>examples</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>in_subset</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>from_schema</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>imported_from</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>in_language</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>see_also</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>deprecated element has exact replacement</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>deprecated element has possible replacement</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>aliases</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>structured_aliases</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>mappings</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>exact mappings</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>close mappings</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>related mappings</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>narrow mappings</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>broad mappings</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>created_by</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>contributors</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>created_on</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>last_updated_on</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>modified_by</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>categories</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>keywords</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"REQUIRED,RECOMMENDED,OPTIONAL,EXAMPLE,DISCOURAGED"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"CODE,CURIE,URI,FHIR_CODING,LABEL"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
release candidate for 1.9.0 series
</commit_message>
<xml_diff>
--- a/linkml_model/excel/meta.xlsx
+++ b/linkml_model/excel/meta.xlsx
@@ -15,30 +15,33 @@
     <sheet name="enum_expression" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="anonymous_enum_expression" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="enum_definition" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="match_query" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="reachability_query" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="structured_alias" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="path_expression" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="anonymous_slot_expression" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="slot_definition" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="anonymous_class_expression" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="class_definition" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="class_rule" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="array_expression" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="dimension_expression" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="pattern_expression" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="import_expression" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="setting" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="prefix" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="local_name" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="example" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="alt_description" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="permissible_value" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="unique_key" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="UnitOfMeasure" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="annotation" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet name="AnyValue" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet name="extension" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="enum_binding" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="match_query" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="reachability_query" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="structured_alias" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="path_expression" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="anonymous_slot_expression" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="slot_definition" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="anonymous_class_expression" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="class_definition" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="class_rule" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="array_expression" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="dimension_expression" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="pattern_expression" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="import_expression" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="setting" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="prefix" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="local_name" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="example" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="alt_description" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="permissible_value" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="unique_key" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="type_mapping" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="extra_slots_expression" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="UnitOfMeasure" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="annotation" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="AnyValue" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="extension" sheetId="35" state="visible" r:id="rId35"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -462,7 +465,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,32 +476,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>identifier_pattern</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>source_ontology</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>source_nodes</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>relationship_types</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>is_direct</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>include_self</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>traverse_up</t>
         </is>
       </c>
     </row>
@@ -513,7 +496,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AK1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -524,6 +507,57 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>source_ontology</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>source_nodes</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>relationship_types</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>is_direct</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>include_self</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>traverse_up</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AL1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>literal_form</t>
         </is>
       </c>
@@ -539,170 +573,175 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>alias_contexts</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>extensions</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>annotations</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>alt_descriptions</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>deprecated</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>todos</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>comments</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>examples</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>in_subset</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>from_schema</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>imported_from</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>source</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>in_language</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>deprecated element has exact replacement</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>deprecated element has possible replacement</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>aliases</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>structured_aliases</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>mappings</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>exact mappings</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>close mappings</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>related mappings</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>narrow mappings</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>broad mappings</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>created_by</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>contributors</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>created_on</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>last_updated_on</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>modified_by</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>rank</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
@@ -718,7 +757,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -954,13 +993,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BJ1"/>
+  <dimension ref="A1:BM1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -986,295 +1025,310 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>bindings</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>required</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>recommended</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>multivalued</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
         <is>
           <t>inlined</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>inlined_as_list</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>minimum_value</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>maximum_value</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>pattern</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>structured_pattern</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>unit</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>implicit_prefix</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>value_presence</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>equals_string</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>equals_string_in</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>equals_number</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>equals_expression</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>exact_cardinality</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>minimum_cardinality</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>maximum_cardinality</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>has_member</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>all_members</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>none_of</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>exactly_one_of</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>any_of</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>all_of</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>array</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
         <is>
           <t>extensions</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>annotations</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>alt_descriptions</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>deprecated</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>todos</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>comments</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>examples</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>in_subset</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>from_schema</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>imported_from</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>source</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>in_language</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>deprecated element has exact replacement</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>deprecated element has possible replacement</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>aliases</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>structured_aliases</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>mappings</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>exact mappings</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>close mappings</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>related mappings</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>narrow mappings</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>broad mappings</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BE1" t="inlineStr">
         <is>
           <t>created_by</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BF1" t="inlineStr">
         <is>
           <t>contributors</t>
         </is>
       </c>
-      <c r="BD1" t="inlineStr">
+      <c r="BG1" t="inlineStr">
         <is>
           <t>created_on</t>
         </is>
       </c>
-      <c r="BE1" t="inlineStr">
+      <c r="BH1" t="inlineStr">
         <is>
           <t>last_updated_on</t>
         </is>
       </c>
-      <c r="BF1" t="inlineStr">
+      <c r="BI1" t="inlineStr">
         <is>
           <t>modified_by</t>
         </is>
       </c>
-      <c r="BG1" t="inlineStr">
+      <c r="BJ1" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
-      <c r="BH1" t="inlineStr">
+      <c r="BK1" t="inlineStr">
         <is>
           <t>rank</t>
         </is>
       </c>
-      <c r="BI1" t="inlineStr">
+      <c r="BL1" t="inlineStr">
         <is>
           <t>categories</t>
         </is>
       </c>
-      <c r="BJ1" t="inlineStr">
+      <c r="BM1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
@@ -1282,7 +1336,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation sqref="N2:N1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="P2:P1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"UNCOMMITTED,PRESENT,ABSENT"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1290,13 +1344,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DK1"/>
+  <dimension ref="A1:DM1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1322,560 +1376,570 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>inherited</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>readonly</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>ifabsent</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>list_elements_unique</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>list_elements_ordered</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>shared</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>key</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>identifier</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>designates_type</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>alias</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>owner</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>domain_of</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>subproperty_of</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>symmetric</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>reflexive</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>locally_reflexive</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>irreflexive</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>asymmetric</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>transitive</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>inverse</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>is_class_field</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>transitive_form_of</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>reflexive_transitive_form_of</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>role</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>is_usage_slot</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>usage_slot_name</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>relational_role</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>slot_group</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>is_grouping_slot</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>path_rule</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>disjoint_with</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>children_are_mutually_disjoint</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>union_of</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>type_mappings</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>range</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>range_expression</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>enum_range</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>bindings</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>required</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>recommended</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
           <t>multivalued</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>inlined</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>inlined_as_list</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
+          <t>minimum_value</t>
+        </is>
+      </c>
+      <c r="AV1" t="inlineStr">
+        <is>
+          <t>maximum_value</t>
+        </is>
+      </c>
+      <c r="AW1" t="inlineStr">
+        <is>
+          <t>pattern</t>
+        </is>
+      </c>
+      <c r="AX1" t="inlineStr">
+        <is>
+          <t>structured_pattern</t>
+        </is>
+      </c>
+      <c r="AY1" t="inlineStr">
+        <is>
+          <t>unit</t>
+        </is>
+      </c>
+      <c r="AZ1" t="inlineStr">
+        <is>
+          <t>implicit_prefix</t>
+        </is>
+      </c>
+      <c r="BA1" t="inlineStr">
+        <is>
+          <t>value_presence</t>
+        </is>
+      </c>
+      <c r="BB1" t="inlineStr">
+        <is>
+          <t>equals_string</t>
+        </is>
+      </c>
+      <c r="BC1" t="inlineStr">
+        <is>
+          <t>equals_string_in</t>
+        </is>
+      </c>
+      <c r="BD1" t="inlineStr">
+        <is>
+          <t>equals_number</t>
+        </is>
+      </c>
+      <c r="BE1" t="inlineStr">
+        <is>
+          <t>equals_expression</t>
+        </is>
+      </c>
+      <c r="BF1" t="inlineStr">
+        <is>
+          <t>exact_cardinality</t>
+        </is>
+      </c>
+      <c r="BG1" t="inlineStr">
+        <is>
+          <t>minimum_cardinality</t>
+        </is>
+      </c>
+      <c r="BH1" t="inlineStr">
+        <is>
+          <t>maximum_cardinality</t>
+        </is>
+      </c>
+      <c r="BI1" t="inlineStr">
+        <is>
+          <t>has_member</t>
+        </is>
+      </c>
+      <c r="BJ1" t="inlineStr">
+        <is>
+          <t>all_members</t>
+        </is>
+      </c>
+      <c r="BK1" t="inlineStr">
+        <is>
+          <t>none_of</t>
+        </is>
+      </c>
+      <c r="BL1" t="inlineStr">
+        <is>
+          <t>exactly_one_of</t>
+        </is>
+      </c>
+      <c r="BM1" t="inlineStr">
+        <is>
+          <t>any_of</t>
+        </is>
+      </c>
+      <c r="BN1" t="inlineStr">
+        <is>
+          <t>all_of</t>
+        </is>
+      </c>
+      <c r="BO1" t="inlineStr">
         <is>
           <t>array</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>inherited</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>readonly</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>ifabsent</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>list_elements_unique</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>list_elements_ordered</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>shared</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>key</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>identifier</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>designates_type</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>alias</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>owner</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>domain_of</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>subproperty_of</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>symmetric</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>reflexive</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>locally_reflexive</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>irreflexive</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>asymmetric</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>transitive</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>inverse</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>is_class_field</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>transitive_form_of</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>reflexive_transitive_form_of</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>role</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>is_usage_slot</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>usage_slot_name</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>relational_role</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>slot_group</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>is_grouping_slot</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>path_rule</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>disjoint_with</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>children_are_mutually_disjoint</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>union_of</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>range</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>range_expression</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>enum_range</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>required</t>
-        </is>
-      </c>
-      <c r="AQ1" t="inlineStr">
-        <is>
-          <t>recommended</t>
-        </is>
-      </c>
-      <c r="AR1" t="inlineStr">
-        <is>
-          <t>inlined</t>
-        </is>
-      </c>
-      <c r="AS1" t="inlineStr">
-        <is>
-          <t>inlined_as_list</t>
-        </is>
-      </c>
-      <c r="AT1" t="inlineStr">
-        <is>
-          <t>minimum_value</t>
-        </is>
-      </c>
-      <c r="AU1" t="inlineStr">
-        <is>
-          <t>maximum_value</t>
-        </is>
-      </c>
-      <c r="AV1" t="inlineStr">
-        <is>
-          <t>pattern</t>
-        </is>
-      </c>
-      <c r="AW1" t="inlineStr">
-        <is>
-          <t>structured_pattern</t>
-        </is>
-      </c>
-      <c r="AX1" t="inlineStr">
-        <is>
-          <t>unit</t>
-        </is>
-      </c>
-      <c r="AY1" t="inlineStr">
-        <is>
-          <t>implicit_prefix</t>
-        </is>
-      </c>
-      <c r="AZ1" t="inlineStr">
-        <is>
-          <t>value_presence</t>
-        </is>
-      </c>
-      <c r="BA1" t="inlineStr">
-        <is>
-          <t>equals_string</t>
-        </is>
-      </c>
-      <c r="BB1" t="inlineStr">
-        <is>
-          <t>equals_string_in</t>
-        </is>
-      </c>
-      <c r="BC1" t="inlineStr">
-        <is>
-          <t>equals_number</t>
-        </is>
-      </c>
-      <c r="BD1" t="inlineStr">
-        <is>
-          <t>equals_expression</t>
-        </is>
-      </c>
-      <c r="BE1" t="inlineStr">
-        <is>
-          <t>exact_cardinality</t>
-        </is>
-      </c>
-      <c r="BF1" t="inlineStr">
-        <is>
-          <t>minimum_cardinality</t>
-        </is>
-      </c>
-      <c r="BG1" t="inlineStr">
-        <is>
-          <t>maximum_cardinality</t>
-        </is>
-      </c>
-      <c r="BH1" t="inlineStr">
-        <is>
-          <t>has_member</t>
-        </is>
-      </c>
-      <c r="BI1" t="inlineStr">
-        <is>
-          <t>all_members</t>
-        </is>
-      </c>
-      <c r="BJ1" t="inlineStr">
-        <is>
-          <t>none_of</t>
-        </is>
-      </c>
-      <c r="BK1" t="inlineStr">
-        <is>
-          <t>exactly_one_of</t>
-        </is>
-      </c>
-      <c r="BL1" t="inlineStr">
-        <is>
-          <t>any_of</t>
-        </is>
-      </c>
-      <c r="BM1" t="inlineStr">
-        <is>
-          <t>all_of</t>
-        </is>
-      </c>
-      <c r="BN1" t="inlineStr">
+      <c r="BP1" t="inlineStr">
         <is>
           <t>is_a</t>
         </is>
       </c>
-      <c r="BO1" t="inlineStr">
+      <c r="BQ1" t="inlineStr">
         <is>
           <t>abstract</t>
         </is>
       </c>
-      <c r="BP1" t="inlineStr">
+      <c r="BR1" t="inlineStr">
         <is>
           <t>mixin</t>
         </is>
       </c>
-      <c r="BQ1" t="inlineStr">
+      <c r="BS1" t="inlineStr">
         <is>
           <t>mixins</t>
         </is>
       </c>
-      <c r="BR1" t="inlineStr">
+      <c r="BT1" t="inlineStr">
         <is>
           <t>apply_to</t>
         </is>
       </c>
-      <c r="BS1" t="inlineStr">
+      <c r="BU1" t="inlineStr">
         <is>
           <t>values_from</t>
         </is>
       </c>
-      <c r="BT1" t="inlineStr">
+      <c r="BV1" t="inlineStr">
         <is>
           <t>string_serialization</t>
         </is>
       </c>
-      <c r="BU1" t="inlineStr">
+      <c r="BW1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="BV1" t="inlineStr">
+      <c r="BX1" t="inlineStr">
         <is>
           <t>id_prefixes</t>
         </is>
       </c>
-      <c r="BW1" t="inlineStr">
+      <c r="BY1" t="inlineStr">
         <is>
           <t>id_prefixes_are_closed</t>
         </is>
       </c>
-      <c r="BX1" t="inlineStr">
+      <c r="BZ1" t="inlineStr">
         <is>
           <t>definition_uri</t>
         </is>
       </c>
-      <c r="BY1" t="inlineStr">
+      <c r="CA1" t="inlineStr">
         <is>
           <t>local_names</t>
         </is>
       </c>
-      <c r="BZ1" t="inlineStr">
+      <c r="CB1" t="inlineStr">
         <is>
           <t>conforms_to</t>
         </is>
       </c>
-      <c r="CA1" t="inlineStr">
+      <c r="CC1" t="inlineStr">
         <is>
           <t>implements</t>
         </is>
       </c>
-      <c r="CB1" t="inlineStr">
+      <c r="CD1" t="inlineStr">
         <is>
           <t>instantiates</t>
         </is>
       </c>
-      <c r="CC1" t="inlineStr">
+      <c r="CE1" t="inlineStr">
         <is>
           <t>extensions</t>
         </is>
       </c>
-      <c r="CD1" t="inlineStr">
+      <c r="CF1" t="inlineStr">
         <is>
           <t>annotations</t>
         </is>
       </c>
-      <c r="CE1" t="inlineStr">
+      <c r="CG1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="CF1" t="inlineStr">
+      <c r="CH1" t="inlineStr">
         <is>
           <t>alt_descriptions</t>
         </is>
       </c>
-      <c r="CG1" t="inlineStr">
+      <c r="CI1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="CH1" t="inlineStr">
+      <c r="CJ1" t="inlineStr">
         <is>
           <t>deprecated</t>
         </is>
       </c>
-      <c r="CI1" t="inlineStr">
+      <c r="CK1" t="inlineStr">
         <is>
           <t>todos</t>
         </is>
       </c>
-      <c r="CJ1" t="inlineStr">
+      <c r="CL1" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
       </c>
-      <c r="CK1" t="inlineStr">
+      <c r="CM1" t="inlineStr">
         <is>
           <t>comments</t>
         </is>
       </c>
-      <c r="CL1" t="inlineStr">
+      <c r="CN1" t="inlineStr">
         <is>
           <t>examples</t>
         </is>
       </c>
-      <c r="CM1" t="inlineStr">
+      <c r="CO1" t="inlineStr">
         <is>
           <t>in_subset</t>
         </is>
       </c>
-      <c r="CN1" t="inlineStr">
+      <c r="CP1" t="inlineStr">
         <is>
           <t>from_schema</t>
         </is>
       </c>
-      <c r="CO1" t="inlineStr">
+      <c r="CQ1" t="inlineStr">
         <is>
           <t>imported_from</t>
         </is>
       </c>
-      <c r="CP1" t="inlineStr">
+      <c r="CR1" t="inlineStr">
         <is>
           <t>source</t>
         </is>
       </c>
-      <c r="CQ1" t="inlineStr">
+      <c r="CS1" t="inlineStr">
         <is>
           <t>in_language</t>
         </is>
       </c>
-      <c r="CR1" t="inlineStr">
+      <c r="CT1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="CS1" t="inlineStr">
+      <c r="CU1" t="inlineStr">
         <is>
           <t>deprecated element has exact replacement</t>
         </is>
       </c>
-      <c r="CT1" t="inlineStr">
+      <c r="CV1" t="inlineStr">
         <is>
           <t>deprecated element has possible replacement</t>
         </is>
       </c>
-      <c r="CU1" t="inlineStr">
+      <c r="CW1" t="inlineStr">
         <is>
           <t>aliases</t>
         </is>
       </c>
-      <c r="CV1" t="inlineStr">
+      <c r="CX1" t="inlineStr">
         <is>
           <t>structured_aliases</t>
         </is>
       </c>
-      <c r="CW1" t="inlineStr">
+      <c r="CY1" t="inlineStr">
         <is>
           <t>mappings</t>
         </is>
       </c>
-      <c r="CX1" t="inlineStr">
+      <c r="CZ1" t="inlineStr">
         <is>
           <t>exact mappings</t>
         </is>
       </c>
-      <c r="CY1" t="inlineStr">
+      <c r="DA1" t="inlineStr">
         <is>
           <t>close mappings</t>
         </is>
       </c>
-      <c r="CZ1" t="inlineStr">
+      <c r="DB1" t="inlineStr">
         <is>
           <t>related mappings</t>
         </is>
       </c>
-      <c r="DA1" t="inlineStr">
+      <c r="DC1" t="inlineStr">
         <is>
           <t>narrow mappings</t>
         </is>
       </c>
-      <c r="DB1" t="inlineStr">
+      <c r="DD1" t="inlineStr">
         <is>
           <t>broad mappings</t>
         </is>
       </c>
-      <c r="DC1" t="inlineStr">
+      <c r="DE1" t="inlineStr">
         <is>
           <t>created_by</t>
         </is>
       </c>
-      <c r="DD1" t="inlineStr">
+      <c r="DF1" t="inlineStr">
         <is>
           <t>contributors</t>
         </is>
       </c>
-      <c r="DE1" t="inlineStr">
+      <c r="DG1" t="inlineStr">
         <is>
           <t>created_on</t>
         </is>
       </c>
-      <c r="DF1" t="inlineStr">
+      <c r="DH1" t="inlineStr">
         <is>
           <t>last_updated_on</t>
         </is>
       </c>
-      <c r="DG1" t="inlineStr">
+      <c r="DI1" t="inlineStr">
         <is>
           <t>modified_by</t>
         </is>
       </c>
-      <c r="DH1" t="inlineStr">
+      <c r="DJ1" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
-      <c r="DI1" t="inlineStr">
+      <c r="DK1" t="inlineStr">
         <is>
           <t>rank</t>
         </is>
       </c>
-      <c r="DJ1" t="inlineStr">
+      <c r="DL1" t="inlineStr">
         <is>
           <t>categories</t>
         </is>
       </c>
-      <c r="DK1" t="inlineStr">
+      <c r="DM1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
@@ -1883,10 +1947,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation sqref="AF2:AF1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="AD2:AD1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"SUBJECT,OBJECT,PREDICATE,NODE,OTHER_ROLE"</formula1>
     </dataValidation>
-    <dataValidation sqref="AZ2:AZ1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="BA2:BA1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"UNCOMMITTED,PRESENT,ABSENT"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1894,7 +1958,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2120,13 +2184,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BR1"/>
+  <dimension ref="A1:BT1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2212,275 +2276,285 @@
       </c>
       <c r="P1" t="inlineStr">
         <is>
+          <t>extra_slots</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>alias</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
           <t>any_of</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>exactly_one_of</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>none_of</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>all_of</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>slot_conditions</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>is_a</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>abstract</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>mixin</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>mixins</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>apply_to</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>values_from</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>string_serialization</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>id_prefixes</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>id_prefixes_are_closed</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>definition_uri</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>local_names</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>conforms_to</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>implements</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>instantiates</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>extensions</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>annotations</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>alt_descriptions</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>deprecated</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>todos</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>comments</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>examples</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>in_subset</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>from_schema</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>imported_from</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>source</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>in_language</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>deprecated element has exact replacement</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>deprecated element has possible replacement</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>aliases</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BE1" t="inlineStr">
         <is>
           <t>structured_aliases</t>
         </is>
       </c>
-      <c r="BD1" t="inlineStr">
+      <c r="BF1" t="inlineStr">
         <is>
           <t>mappings</t>
         </is>
       </c>
-      <c r="BE1" t="inlineStr">
+      <c r="BG1" t="inlineStr">
         <is>
           <t>exact mappings</t>
         </is>
       </c>
-      <c r="BF1" t="inlineStr">
+      <c r="BH1" t="inlineStr">
         <is>
           <t>close mappings</t>
         </is>
       </c>
-      <c r="BG1" t="inlineStr">
+      <c r="BI1" t="inlineStr">
         <is>
           <t>related mappings</t>
         </is>
       </c>
-      <c r="BH1" t="inlineStr">
+      <c r="BJ1" t="inlineStr">
         <is>
           <t>narrow mappings</t>
         </is>
       </c>
-      <c r="BI1" t="inlineStr">
+      <c r="BK1" t="inlineStr">
         <is>
           <t>broad mappings</t>
         </is>
       </c>
-      <c r="BJ1" t="inlineStr">
+      <c r="BL1" t="inlineStr">
         <is>
           <t>created_by</t>
         </is>
       </c>
-      <c r="BK1" t="inlineStr">
+      <c r="BM1" t="inlineStr">
         <is>
           <t>contributors</t>
         </is>
       </c>
-      <c r="BL1" t="inlineStr">
+      <c r="BN1" t="inlineStr">
         <is>
           <t>created_on</t>
         </is>
       </c>
-      <c r="BM1" t="inlineStr">
+      <c r="BO1" t="inlineStr">
         <is>
           <t>last_updated_on</t>
         </is>
       </c>
-      <c r="BN1" t="inlineStr">
+      <c r="BP1" t="inlineStr">
         <is>
           <t>modified_by</t>
         </is>
       </c>
-      <c r="BO1" t="inlineStr">
+      <c r="BQ1" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
-      <c r="BP1" t="inlineStr">
+      <c r="BR1" t="inlineStr">
         <is>
           <t>rank</t>
         </is>
       </c>
-      <c r="BQ1" t="inlineStr">
+      <c r="BS1" t="inlineStr">
         <is>
           <t>categories</t>
         </is>
       </c>
-      <c r="BR1" t="inlineStr">
+      <c r="BT1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
@@ -2491,7 +2565,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2707,227 +2781,6 @@
         </is>
       </c>
       <c r="AO1" t="inlineStr">
-        <is>
-          <t>keywords</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AN1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>exact_number_dimensions</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>minimum_number_dimensions</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>maximum_number_dimensions</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>has_extra_dimensions</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>dimensions</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>extensions</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>annotations</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>alt_descriptions</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>deprecated</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>todos</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>notes</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>comments</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>examples</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>in_subset</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>from_schema</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>imported_from</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>source</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>in_language</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>see_also</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>deprecated element has exact replacement</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>deprecated element has possible replacement</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>aliases</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>structured_aliases</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>mappings</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>exact mappings</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>close mappings</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>related mappings</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>narrow mappings</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>broad mappings</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>created_by</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>contributors</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>created_on</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>last_updated_on</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>modified_by</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>status</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>rank</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>categories</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
@@ -2955,22 +2808,22 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>alias</t>
+          <t>exact_number_dimensions</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>maximum_cardinality</t>
+          <t>minimum_number_dimensions</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>minimum_cardinality</t>
+          <t>maximum_number_dimensions</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>exact_cardinality</t>
+          <t>dimensions</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
@@ -3160,7 +3013,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BL1"/>
+  <dimension ref="A1:BM1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3276,215 +3129,220 @@
       </c>
       <c r="V1" t="inlineStr">
         <is>
+          <t>bindings</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
           <t>name</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>id_prefixes</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>id_prefixes_are_closed</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>definition_uri</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>local_names</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>conforms_to</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>implements</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>instantiates</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>extensions</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>annotations</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>alt_descriptions</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>deprecated</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>todos</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>comments</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>examples</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>in_subset</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>from_schema</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>imported_from</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>source</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>in_language</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>deprecated element has exact replacement</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>deprecated element has possible replacement</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>aliases</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>structured_aliases</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>mappings</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>exact mappings</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>close mappings</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>related mappings</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>narrow mappings</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>broad mappings</t>
         </is>
       </c>
-      <c r="BD1" t="inlineStr">
+      <c r="BE1" t="inlineStr">
         <is>
           <t>created_by</t>
         </is>
       </c>
-      <c r="BE1" t="inlineStr">
+      <c r="BF1" t="inlineStr">
         <is>
           <t>contributors</t>
         </is>
       </c>
-      <c r="BF1" t="inlineStr">
+      <c r="BG1" t="inlineStr">
         <is>
           <t>created_on</t>
         </is>
       </c>
-      <c r="BG1" t="inlineStr">
+      <c r="BH1" t="inlineStr">
         <is>
           <t>last_updated_on</t>
         </is>
       </c>
-      <c r="BH1" t="inlineStr">
+      <c r="BI1" t="inlineStr">
         <is>
           <t>modified_by</t>
         </is>
       </c>
-      <c r="BI1" t="inlineStr">
+      <c r="BJ1" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
-      <c r="BJ1" t="inlineStr">
+      <c r="BK1" t="inlineStr">
         <is>
           <t>rank</t>
         </is>
       </c>
-      <c r="BK1" t="inlineStr">
+      <c r="BL1" t="inlineStr">
         <is>
           <t>categories</t>
         </is>
       </c>
-      <c r="BL1" t="inlineStr">
+      <c r="BM1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
@@ -3501,7 +3359,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AL1"/>
+  <dimension ref="A1:AM1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3512,190 +3370,195 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>syntax</t>
+          <t>alias</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>interpolated</t>
+          <t>maximum_cardinality</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>partial_match</t>
+          <t>minimum_cardinality</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>exact_cardinality</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>extensions</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>annotations</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>alt_descriptions</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>deprecated</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>todos</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>comments</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>examples</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>in_subset</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>from_schema</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>imported_from</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>source</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>in_language</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>deprecated element has exact replacement</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>deprecated element has possible replacement</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>aliases</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>structured_aliases</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>mappings</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>exact mappings</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>close mappings</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>related mappings</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>narrow mappings</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>broad mappings</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>created_by</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>contributors</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>created_on</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>last_updated_on</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>modified_by</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>rank</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>categories</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
@@ -3723,17 +3586,17 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>import_from</t>
+          <t>syntax</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>import_as</t>
+          <t>interpolated</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>import_map</t>
+          <t>partial_match</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -3923,7 +3786,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:AL1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3934,12 +3797,192 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>setting_key</t>
+          <t>import_from</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>setting_value</t>
+          <t>import_as</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>import_map</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>extensions</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>annotations</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>alt_descriptions</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>deprecated</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>todos</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>notes</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>examples</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>in_subset</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>from_schema</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>imported_from</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>in_language</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>see_also</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>deprecated element has exact replacement</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>deprecated element has possible replacement</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>aliases</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>structured_aliases</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>mappings</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>exact mappings</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>close mappings</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>related mappings</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>narrow mappings</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>broad mappings</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>created_by</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>contributors</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>created_on</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>last_updated_on</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>modified_by</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>categories</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>keywords</t>
         </is>
       </c>
     </row>
@@ -3965,12 +4008,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>prefix_prefix</t>
+          <t>setting_key</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>prefix_reference</t>
+          <t>setting_value</t>
         </is>
       </c>
     </row>
@@ -3996,12 +4039,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>local_name_source</t>
+          <t>prefix_prefix</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>local_name_value</t>
+          <t>prefix_reference</t>
         </is>
       </c>
     </row>
@@ -4011,6 +4054,37 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>local_name_source</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>local_name_value</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4046,7 +4120,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4077,7 +4151,238 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AP1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>meaning</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>unit</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>instantiates</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>implements</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>is_a</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>mixins</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>extensions</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>annotations</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>alt_descriptions</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>deprecated</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>todos</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>notes</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>examples</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>in_subset</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>from_schema</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>imported_from</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>in_language</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>see_also</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>deprecated element has exact replacement</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>deprecated element has possible replacement</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>aliases</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>structured_aliases</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>mappings</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>exact mappings</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>close mappings</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>related mappings</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>narrow mappings</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>broad mappings</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>created_by</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>contributors</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>created_on</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>last_updated_on</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>modified_by</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>categories</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>keywords</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4094,34 +4399,34 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>unique_key_name</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>unique_key_slots</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>consider_nulls_inequal</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>extensions</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>annotations</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>description</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>meaning</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>unit</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>extensions</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>annotations</t>
-        </is>
-      </c>
       <c r="G1" t="inlineStr">
         <is>
           <t>alt_descriptions</t>
@@ -4280,278 +4585,6 @@
       <c r="AL1" t="inlineStr">
         <is>
           <t>keywords</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AL1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>unique_key_name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>unique_key_slots</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>consider_nulls_inequal</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>extensions</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>annotations</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>alt_descriptions</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>deprecated</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>todos</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>notes</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>comments</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>examples</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>in_subset</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>from_schema</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>imported_from</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>source</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>in_language</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>see_also</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>deprecated element has exact replacement</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>deprecated element has possible replacement</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>aliases</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>structured_aliases</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>mappings</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>exact mappings</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>close mappings</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>related mappings</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>narrow mappings</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>broad mappings</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>created_by</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>contributors</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>created_on</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>last_updated_on</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>modified_by</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>status</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>rank</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>categories</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>keywords</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>symbol</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>abbreviation</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>descriptive_name</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>exact mappings</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>ucum_code</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>derivation</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>has_quantity_kind</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>iec61360code</t>
         </is>
       </c>
     </row>
@@ -4652,6 +4685,309 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:AL1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>framework_key</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>mapped_type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>string_serialization</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>extensions</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>annotations</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>alt_descriptions</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>deprecated</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>todos</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>notes</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>examples</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>in_subset</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>from_schema</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>imported_from</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>in_language</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>see_also</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>deprecated element has exact replacement</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>deprecated element has possible replacement</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>aliases</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>structured_aliases</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>mappings</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>exact mappings</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>close mappings</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>related mappings</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>narrow mappings</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>broad mappings</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>created_by</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>contributors</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>created_on</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>last_updated_on</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>modified_by</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>categories</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>keywords</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>allowed</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>range_expression</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>symbol</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>abbreviation</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>descriptive_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>exact mappings</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>ucum_code</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>derivation</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>has_quantity_kind</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>iec61360code</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4687,7 +5023,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4705,7 +5041,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -5807,7 +6143,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:AM1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5818,16 +6154,209 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>identifier_pattern</t>
+          <t>range</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>source_ontology</t>
+          <t>obligation_level</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>binds_value_of</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>pv_formula</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>extensions</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>annotations</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>alt_descriptions</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>deprecated</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>todos</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>notes</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>examples</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>in_subset</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>from_schema</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>imported_from</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>in_language</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>see_also</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>deprecated element has exact replacement</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>deprecated element has possible replacement</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>aliases</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>structured_aliases</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>mappings</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>exact mappings</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>close mappings</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>related mappings</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>narrow mappings</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>broad mappings</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>created_by</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>contributors</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>created_on</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>last_updated_on</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>modified_by</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>categories</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>keywords</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"REQUIRED,RECOMMENDED,OPTIONAL,EXAMPLE,DISCOURAGED"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"CODE,CURIE,URI,FHIR_CODING,LABEL"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
regenerated with latest linkml
</commit_message>
<xml_diff>
--- a/linkml_model/excel/meta.xlsx
+++ b/linkml_model/excel/meta.xlsx
@@ -15,30 +15,33 @@
     <sheet name="enum_expression" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="anonymous_enum_expression" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="enum_definition" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="match_query" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="reachability_query" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="structured_alias" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="path_expression" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="anonymous_slot_expression" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="slot_definition" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="anonymous_class_expression" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="class_definition" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="class_rule" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="array_expression" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="dimension_expression" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="pattern_expression" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="import_expression" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="setting" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="prefix" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="local_name" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="example" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="alt_description" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="permissible_value" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="unique_key" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="UnitOfMeasure" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="annotation" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet name="AnyValue" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet name="extension" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="enum_binding" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="match_query" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="reachability_query" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="structured_alias" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="path_expression" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="anonymous_slot_expression" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="slot_definition" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="anonymous_class_expression" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="class_definition" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="class_rule" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="array_expression" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="dimension_expression" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="pattern_expression" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="import_expression" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="setting" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="prefix" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="local_name" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="example" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="alt_description" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="permissible_value" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="unique_key" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="type_mapping" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="extra_slots_expression" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="UnitOfMeasure" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="annotation" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="AnyValue" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="extension" sheetId="35" state="visible" r:id="rId35"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -462,7 +465,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,32 +476,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>identifier_pattern</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>source_ontology</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>source_nodes</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>relationship_types</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>is_direct</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>include_self</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>traverse_up</t>
         </is>
       </c>
     </row>
@@ -513,7 +496,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AK1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -524,6 +507,57 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>source_ontology</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>source_nodes</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>relationship_types</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>is_direct</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>include_self</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>traverse_up</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AL1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>literal_form</t>
         </is>
       </c>
@@ -539,170 +573,175 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>alias_contexts</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>extensions</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>annotations</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>alt_descriptions</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>deprecated</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>todos</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>comments</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>examples</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>in_subset</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>from_schema</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>imported_from</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>source</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>in_language</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>deprecated element has exact replacement</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>deprecated element has possible replacement</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>aliases</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>structured_aliases</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>mappings</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>exact mappings</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>close mappings</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>related mappings</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>narrow mappings</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>broad mappings</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>created_by</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>contributors</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>created_on</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>last_updated_on</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>modified_by</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>rank</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
@@ -718,7 +757,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -954,13 +993,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BJ1"/>
+  <dimension ref="A1:BM1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -986,295 +1025,310 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>bindings</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>required</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>recommended</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>multivalued</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
         <is>
           <t>inlined</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>inlined_as_list</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>minimum_value</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>maximum_value</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>pattern</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>structured_pattern</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>unit</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>implicit_prefix</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>value_presence</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>equals_string</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>equals_string_in</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>equals_number</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>equals_expression</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>exact_cardinality</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>minimum_cardinality</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>maximum_cardinality</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>has_member</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>all_members</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>none_of</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>exactly_one_of</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>any_of</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>all_of</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>array</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
         <is>
           <t>extensions</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>annotations</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>alt_descriptions</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>deprecated</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>todos</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>comments</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>examples</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>in_subset</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>from_schema</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>imported_from</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>source</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>in_language</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>deprecated element has exact replacement</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>deprecated element has possible replacement</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>aliases</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>structured_aliases</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>mappings</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>exact mappings</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>close mappings</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>related mappings</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>narrow mappings</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>broad mappings</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BE1" t="inlineStr">
         <is>
           <t>created_by</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BF1" t="inlineStr">
         <is>
           <t>contributors</t>
         </is>
       </c>
-      <c r="BD1" t="inlineStr">
+      <c r="BG1" t="inlineStr">
         <is>
           <t>created_on</t>
         </is>
       </c>
-      <c r="BE1" t="inlineStr">
+      <c r="BH1" t="inlineStr">
         <is>
           <t>last_updated_on</t>
         </is>
       </c>
-      <c r="BF1" t="inlineStr">
+      <c r="BI1" t="inlineStr">
         <is>
           <t>modified_by</t>
         </is>
       </c>
-      <c r="BG1" t="inlineStr">
+      <c r="BJ1" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
-      <c r="BH1" t="inlineStr">
+      <c r="BK1" t="inlineStr">
         <is>
           <t>rank</t>
         </is>
       </c>
-      <c r="BI1" t="inlineStr">
+      <c r="BL1" t="inlineStr">
         <is>
           <t>categories</t>
         </is>
       </c>
-      <c r="BJ1" t="inlineStr">
+      <c r="BM1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
@@ -1282,7 +1336,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation sqref="N2:N1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="P2:P1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"UNCOMMITTED,PRESENT,ABSENT"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1290,13 +1344,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DK1"/>
+  <dimension ref="A1:DM1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1322,560 +1376,570 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>inherited</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>readonly</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>ifabsent</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>list_elements_unique</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>list_elements_ordered</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>shared</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>key</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>identifier</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>designates_type</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>alias</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>owner</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>domain_of</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>subproperty_of</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>symmetric</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>reflexive</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>locally_reflexive</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>irreflexive</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>asymmetric</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>transitive</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>inverse</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>is_class_field</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>transitive_form_of</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>reflexive_transitive_form_of</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>role</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>is_usage_slot</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>usage_slot_name</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>relational_role</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>slot_group</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>is_grouping_slot</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>path_rule</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>disjoint_with</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>children_are_mutually_disjoint</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>union_of</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>type_mappings</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>range</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>range_expression</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>enum_range</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>bindings</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>required</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>recommended</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
           <t>multivalued</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>inlined</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>inlined_as_list</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
+          <t>minimum_value</t>
+        </is>
+      </c>
+      <c r="AV1" t="inlineStr">
+        <is>
+          <t>maximum_value</t>
+        </is>
+      </c>
+      <c r="AW1" t="inlineStr">
+        <is>
+          <t>pattern</t>
+        </is>
+      </c>
+      <c r="AX1" t="inlineStr">
+        <is>
+          <t>structured_pattern</t>
+        </is>
+      </c>
+      <c r="AY1" t="inlineStr">
+        <is>
+          <t>unit</t>
+        </is>
+      </c>
+      <c r="AZ1" t="inlineStr">
+        <is>
+          <t>implicit_prefix</t>
+        </is>
+      </c>
+      <c r="BA1" t="inlineStr">
+        <is>
+          <t>value_presence</t>
+        </is>
+      </c>
+      <c r="BB1" t="inlineStr">
+        <is>
+          <t>equals_string</t>
+        </is>
+      </c>
+      <c r="BC1" t="inlineStr">
+        <is>
+          <t>equals_string_in</t>
+        </is>
+      </c>
+      <c r="BD1" t="inlineStr">
+        <is>
+          <t>equals_number</t>
+        </is>
+      </c>
+      <c r="BE1" t="inlineStr">
+        <is>
+          <t>equals_expression</t>
+        </is>
+      </c>
+      <c r="BF1" t="inlineStr">
+        <is>
+          <t>exact_cardinality</t>
+        </is>
+      </c>
+      <c r="BG1" t="inlineStr">
+        <is>
+          <t>minimum_cardinality</t>
+        </is>
+      </c>
+      <c r="BH1" t="inlineStr">
+        <is>
+          <t>maximum_cardinality</t>
+        </is>
+      </c>
+      <c r="BI1" t="inlineStr">
+        <is>
+          <t>has_member</t>
+        </is>
+      </c>
+      <c r="BJ1" t="inlineStr">
+        <is>
+          <t>all_members</t>
+        </is>
+      </c>
+      <c r="BK1" t="inlineStr">
+        <is>
+          <t>none_of</t>
+        </is>
+      </c>
+      <c r="BL1" t="inlineStr">
+        <is>
+          <t>exactly_one_of</t>
+        </is>
+      </c>
+      <c r="BM1" t="inlineStr">
+        <is>
+          <t>any_of</t>
+        </is>
+      </c>
+      <c r="BN1" t="inlineStr">
+        <is>
+          <t>all_of</t>
+        </is>
+      </c>
+      <c r="BO1" t="inlineStr">
         <is>
           <t>array</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>inherited</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>readonly</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>ifabsent</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>list_elements_unique</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>list_elements_ordered</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>shared</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>key</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>identifier</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>designates_type</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>alias</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>owner</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>domain_of</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>subproperty_of</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>symmetric</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>reflexive</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>locally_reflexive</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>irreflexive</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>asymmetric</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>transitive</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>inverse</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>is_class_field</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>transitive_form_of</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>reflexive_transitive_form_of</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>role</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>is_usage_slot</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>usage_slot_name</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>relational_role</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>slot_group</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>is_grouping_slot</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>path_rule</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>disjoint_with</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>children_are_mutually_disjoint</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>union_of</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>range</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>range_expression</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>enum_range</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>required</t>
-        </is>
-      </c>
-      <c r="AQ1" t="inlineStr">
-        <is>
-          <t>recommended</t>
-        </is>
-      </c>
-      <c r="AR1" t="inlineStr">
-        <is>
-          <t>inlined</t>
-        </is>
-      </c>
-      <c r="AS1" t="inlineStr">
-        <is>
-          <t>inlined_as_list</t>
-        </is>
-      </c>
-      <c r="AT1" t="inlineStr">
-        <is>
-          <t>minimum_value</t>
-        </is>
-      </c>
-      <c r="AU1" t="inlineStr">
-        <is>
-          <t>maximum_value</t>
-        </is>
-      </c>
-      <c r="AV1" t="inlineStr">
-        <is>
-          <t>pattern</t>
-        </is>
-      </c>
-      <c r="AW1" t="inlineStr">
-        <is>
-          <t>structured_pattern</t>
-        </is>
-      </c>
-      <c r="AX1" t="inlineStr">
-        <is>
-          <t>unit</t>
-        </is>
-      </c>
-      <c r="AY1" t="inlineStr">
-        <is>
-          <t>implicit_prefix</t>
-        </is>
-      </c>
-      <c r="AZ1" t="inlineStr">
-        <is>
-          <t>value_presence</t>
-        </is>
-      </c>
-      <c r="BA1" t="inlineStr">
-        <is>
-          <t>equals_string</t>
-        </is>
-      </c>
-      <c r="BB1" t="inlineStr">
-        <is>
-          <t>equals_string_in</t>
-        </is>
-      </c>
-      <c r="BC1" t="inlineStr">
-        <is>
-          <t>equals_number</t>
-        </is>
-      </c>
-      <c r="BD1" t="inlineStr">
-        <is>
-          <t>equals_expression</t>
-        </is>
-      </c>
-      <c r="BE1" t="inlineStr">
-        <is>
-          <t>exact_cardinality</t>
-        </is>
-      </c>
-      <c r="BF1" t="inlineStr">
-        <is>
-          <t>minimum_cardinality</t>
-        </is>
-      </c>
-      <c r="BG1" t="inlineStr">
-        <is>
-          <t>maximum_cardinality</t>
-        </is>
-      </c>
-      <c r="BH1" t="inlineStr">
-        <is>
-          <t>has_member</t>
-        </is>
-      </c>
-      <c r="BI1" t="inlineStr">
-        <is>
-          <t>all_members</t>
-        </is>
-      </c>
-      <c r="BJ1" t="inlineStr">
-        <is>
-          <t>none_of</t>
-        </is>
-      </c>
-      <c r="BK1" t="inlineStr">
-        <is>
-          <t>exactly_one_of</t>
-        </is>
-      </c>
-      <c r="BL1" t="inlineStr">
-        <is>
-          <t>any_of</t>
-        </is>
-      </c>
-      <c r="BM1" t="inlineStr">
-        <is>
-          <t>all_of</t>
-        </is>
-      </c>
-      <c r="BN1" t="inlineStr">
+      <c r="BP1" t="inlineStr">
         <is>
           <t>is_a</t>
         </is>
       </c>
-      <c r="BO1" t="inlineStr">
+      <c r="BQ1" t="inlineStr">
         <is>
           <t>abstract</t>
         </is>
       </c>
-      <c r="BP1" t="inlineStr">
+      <c r="BR1" t="inlineStr">
         <is>
           <t>mixin</t>
         </is>
       </c>
-      <c r="BQ1" t="inlineStr">
+      <c r="BS1" t="inlineStr">
         <is>
           <t>mixins</t>
         </is>
       </c>
-      <c r="BR1" t="inlineStr">
+      <c r="BT1" t="inlineStr">
         <is>
           <t>apply_to</t>
         </is>
       </c>
-      <c r="BS1" t="inlineStr">
+      <c r="BU1" t="inlineStr">
         <is>
           <t>values_from</t>
         </is>
       </c>
-      <c r="BT1" t="inlineStr">
+      <c r="BV1" t="inlineStr">
         <is>
           <t>string_serialization</t>
         </is>
       </c>
-      <c r="BU1" t="inlineStr">
+      <c r="BW1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="BV1" t="inlineStr">
+      <c r="BX1" t="inlineStr">
         <is>
           <t>id_prefixes</t>
         </is>
       </c>
-      <c r="BW1" t="inlineStr">
+      <c r="BY1" t="inlineStr">
         <is>
           <t>id_prefixes_are_closed</t>
         </is>
       </c>
-      <c r="BX1" t="inlineStr">
+      <c r="BZ1" t="inlineStr">
         <is>
           <t>definition_uri</t>
         </is>
       </c>
-      <c r="BY1" t="inlineStr">
+      <c r="CA1" t="inlineStr">
         <is>
           <t>local_names</t>
         </is>
       </c>
-      <c r="BZ1" t="inlineStr">
+      <c r="CB1" t="inlineStr">
         <is>
           <t>conforms_to</t>
         </is>
       </c>
-      <c r="CA1" t="inlineStr">
+      <c r="CC1" t="inlineStr">
         <is>
           <t>implements</t>
         </is>
       </c>
-      <c r="CB1" t="inlineStr">
+      <c r="CD1" t="inlineStr">
         <is>
           <t>instantiates</t>
         </is>
       </c>
-      <c r="CC1" t="inlineStr">
+      <c r="CE1" t="inlineStr">
         <is>
           <t>extensions</t>
         </is>
       </c>
-      <c r="CD1" t="inlineStr">
+      <c r="CF1" t="inlineStr">
         <is>
           <t>annotations</t>
         </is>
       </c>
-      <c r="CE1" t="inlineStr">
+      <c r="CG1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="CF1" t="inlineStr">
+      <c r="CH1" t="inlineStr">
         <is>
           <t>alt_descriptions</t>
         </is>
       </c>
-      <c r="CG1" t="inlineStr">
+      <c r="CI1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="CH1" t="inlineStr">
+      <c r="CJ1" t="inlineStr">
         <is>
           <t>deprecated</t>
         </is>
       </c>
-      <c r="CI1" t="inlineStr">
+      <c r="CK1" t="inlineStr">
         <is>
           <t>todos</t>
         </is>
       </c>
-      <c r="CJ1" t="inlineStr">
+      <c r="CL1" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
       </c>
-      <c r="CK1" t="inlineStr">
+      <c r="CM1" t="inlineStr">
         <is>
           <t>comments</t>
         </is>
       </c>
-      <c r="CL1" t="inlineStr">
+      <c r="CN1" t="inlineStr">
         <is>
           <t>examples</t>
         </is>
       </c>
-      <c r="CM1" t="inlineStr">
+      <c r="CO1" t="inlineStr">
         <is>
           <t>in_subset</t>
         </is>
       </c>
-      <c r="CN1" t="inlineStr">
+      <c r="CP1" t="inlineStr">
         <is>
           <t>from_schema</t>
         </is>
       </c>
-      <c r="CO1" t="inlineStr">
+      <c r="CQ1" t="inlineStr">
         <is>
           <t>imported_from</t>
         </is>
       </c>
-      <c r="CP1" t="inlineStr">
+      <c r="CR1" t="inlineStr">
         <is>
           <t>source</t>
         </is>
       </c>
-      <c r="CQ1" t="inlineStr">
+      <c r="CS1" t="inlineStr">
         <is>
           <t>in_language</t>
         </is>
       </c>
-      <c r="CR1" t="inlineStr">
+      <c r="CT1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="CS1" t="inlineStr">
+      <c r="CU1" t="inlineStr">
         <is>
           <t>deprecated element has exact replacement</t>
         </is>
       </c>
-      <c r="CT1" t="inlineStr">
+      <c r="CV1" t="inlineStr">
         <is>
           <t>deprecated element has possible replacement</t>
         </is>
       </c>
-      <c r="CU1" t="inlineStr">
+      <c r="CW1" t="inlineStr">
         <is>
           <t>aliases</t>
         </is>
       </c>
-      <c r="CV1" t="inlineStr">
+      <c r="CX1" t="inlineStr">
         <is>
           <t>structured_aliases</t>
         </is>
       </c>
-      <c r="CW1" t="inlineStr">
+      <c r="CY1" t="inlineStr">
         <is>
           <t>mappings</t>
         </is>
       </c>
-      <c r="CX1" t="inlineStr">
+      <c r="CZ1" t="inlineStr">
         <is>
           <t>exact mappings</t>
         </is>
       </c>
-      <c r="CY1" t="inlineStr">
+      <c r="DA1" t="inlineStr">
         <is>
           <t>close mappings</t>
         </is>
       </c>
-      <c r="CZ1" t="inlineStr">
+      <c r="DB1" t="inlineStr">
         <is>
           <t>related mappings</t>
         </is>
       </c>
-      <c r="DA1" t="inlineStr">
+      <c r="DC1" t="inlineStr">
         <is>
           <t>narrow mappings</t>
         </is>
       </c>
-      <c r="DB1" t="inlineStr">
+      <c r="DD1" t="inlineStr">
         <is>
           <t>broad mappings</t>
         </is>
       </c>
-      <c r="DC1" t="inlineStr">
+      <c r="DE1" t="inlineStr">
         <is>
           <t>created_by</t>
         </is>
       </c>
-      <c r="DD1" t="inlineStr">
+      <c r="DF1" t="inlineStr">
         <is>
           <t>contributors</t>
         </is>
       </c>
-      <c r="DE1" t="inlineStr">
+      <c r="DG1" t="inlineStr">
         <is>
           <t>created_on</t>
         </is>
       </c>
-      <c r="DF1" t="inlineStr">
+      <c r="DH1" t="inlineStr">
         <is>
           <t>last_updated_on</t>
         </is>
       </c>
-      <c r="DG1" t="inlineStr">
+      <c r="DI1" t="inlineStr">
         <is>
           <t>modified_by</t>
         </is>
       </c>
-      <c r="DH1" t="inlineStr">
+      <c r="DJ1" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
-      <c r="DI1" t="inlineStr">
+      <c r="DK1" t="inlineStr">
         <is>
           <t>rank</t>
         </is>
       </c>
-      <c r="DJ1" t="inlineStr">
+      <c r="DL1" t="inlineStr">
         <is>
           <t>categories</t>
         </is>
       </c>
-      <c r="DK1" t="inlineStr">
+      <c r="DM1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
@@ -1883,10 +1947,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation sqref="AF2:AF1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="AD2:AD1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"SUBJECT,OBJECT,PREDICATE,NODE,OTHER_ROLE"</formula1>
     </dataValidation>
-    <dataValidation sqref="AZ2:AZ1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="BA2:BA1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"UNCOMMITTED,PRESENT,ABSENT"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1894,7 +1958,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2120,13 +2184,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BR1"/>
+  <dimension ref="A1:BT1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2212,275 +2276,285 @@
       </c>
       <c r="P1" t="inlineStr">
         <is>
+          <t>extra_slots</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>alias</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
           <t>any_of</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>exactly_one_of</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>none_of</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>all_of</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>slot_conditions</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>is_a</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>abstract</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>mixin</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>mixins</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>apply_to</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>values_from</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>string_serialization</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>id_prefixes</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>id_prefixes_are_closed</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>definition_uri</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>local_names</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>conforms_to</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>implements</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>instantiates</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>extensions</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>annotations</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>alt_descriptions</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>deprecated</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>todos</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>comments</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>examples</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>in_subset</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>from_schema</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>imported_from</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>source</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>in_language</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>deprecated element has exact replacement</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>deprecated element has possible replacement</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>aliases</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BE1" t="inlineStr">
         <is>
           <t>structured_aliases</t>
         </is>
       </c>
-      <c r="BD1" t="inlineStr">
+      <c r="BF1" t="inlineStr">
         <is>
           <t>mappings</t>
         </is>
       </c>
-      <c r="BE1" t="inlineStr">
+      <c r="BG1" t="inlineStr">
         <is>
           <t>exact mappings</t>
         </is>
       </c>
-      <c r="BF1" t="inlineStr">
+      <c r="BH1" t="inlineStr">
         <is>
           <t>close mappings</t>
         </is>
       </c>
-      <c r="BG1" t="inlineStr">
+      <c r="BI1" t="inlineStr">
         <is>
           <t>related mappings</t>
         </is>
       </c>
-      <c r="BH1" t="inlineStr">
+      <c r="BJ1" t="inlineStr">
         <is>
           <t>narrow mappings</t>
         </is>
       </c>
-      <c r="BI1" t="inlineStr">
+      <c r="BK1" t="inlineStr">
         <is>
           <t>broad mappings</t>
         </is>
       </c>
-      <c r="BJ1" t="inlineStr">
+      <c r="BL1" t="inlineStr">
         <is>
           <t>created_by</t>
         </is>
       </c>
-      <c r="BK1" t="inlineStr">
+      <c r="BM1" t="inlineStr">
         <is>
           <t>contributors</t>
         </is>
       </c>
-      <c r="BL1" t="inlineStr">
+      <c r="BN1" t="inlineStr">
         <is>
           <t>created_on</t>
         </is>
       </c>
-      <c r="BM1" t="inlineStr">
+      <c r="BO1" t="inlineStr">
         <is>
           <t>last_updated_on</t>
         </is>
       </c>
-      <c r="BN1" t="inlineStr">
+      <c r="BP1" t="inlineStr">
         <is>
           <t>modified_by</t>
         </is>
       </c>
-      <c r="BO1" t="inlineStr">
+      <c r="BQ1" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
-      <c r="BP1" t="inlineStr">
+      <c r="BR1" t="inlineStr">
         <is>
           <t>rank</t>
         </is>
       </c>
-      <c r="BQ1" t="inlineStr">
+      <c r="BS1" t="inlineStr">
         <is>
           <t>categories</t>
         </is>
       </c>
-      <c r="BR1" t="inlineStr">
+      <c r="BT1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
@@ -2491,7 +2565,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2707,227 +2781,6 @@
         </is>
       </c>
       <c r="AO1" t="inlineStr">
-        <is>
-          <t>keywords</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AN1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>exact_number_dimensions</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>minimum_number_dimensions</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>maximum_number_dimensions</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>has_extra_dimensions</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>dimensions</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>extensions</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>annotations</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>alt_descriptions</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>deprecated</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>todos</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>notes</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>comments</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>examples</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>in_subset</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>from_schema</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>imported_from</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>source</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>in_language</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>see_also</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>deprecated element has exact replacement</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>deprecated element has possible replacement</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>aliases</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>structured_aliases</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>mappings</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>exact mappings</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>close mappings</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>related mappings</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>narrow mappings</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>broad mappings</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>created_by</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>contributors</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>created_on</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>last_updated_on</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>modified_by</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>status</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>rank</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>categories</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
@@ -2955,22 +2808,22 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>alias</t>
+          <t>exact_number_dimensions</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>maximum_cardinality</t>
+          <t>minimum_number_dimensions</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>minimum_cardinality</t>
+          <t>maximum_number_dimensions</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>exact_cardinality</t>
+          <t>dimensions</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
@@ -3160,7 +3013,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BL1"/>
+  <dimension ref="A1:BM1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3276,215 +3129,220 @@
       </c>
       <c r="V1" t="inlineStr">
         <is>
+          <t>bindings</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
           <t>name</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>id_prefixes</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>id_prefixes_are_closed</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>definition_uri</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>local_names</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>conforms_to</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>implements</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>instantiates</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>extensions</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>annotations</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>alt_descriptions</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>deprecated</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>todos</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>comments</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>examples</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>in_subset</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>from_schema</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>imported_from</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>source</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>in_language</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>deprecated element has exact replacement</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>deprecated element has possible replacement</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>aliases</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>structured_aliases</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>mappings</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>exact mappings</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>close mappings</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>related mappings</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>narrow mappings</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>broad mappings</t>
         </is>
       </c>
-      <c r="BD1" t="inlineStr">
+      <c r="BE1" t="inlineStr">
         <is>
           <t>created_by</t>
         </is>
       </c>
-      <c r="BE1" t="inlineStr">
+      <c r="BF1" t="inlineStr">
         <is>
           <t>contributors</t>
         </is>
       </c>
-      <c r="BF1" t="inlineStr">
+      <c r="BG1" t="inlineStr">
         <is>
           <t>created_on</t>
         </is>
       </c>
-      <c r="BG1" t="inlineStr">
+      <c r="BH1" t="inlineStr">
         <is>
           <t>last_updated_on</t>
         </is>
       </c>
-      <c r="BH1" t="inlineStr">
+      <c r="BI1" t="inlineStr">
         <is>
           <t>modified_by</t>
         </is>
       </c>
-      <c r="BI1" t="inlineStr">
+      <c r="BJ1" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
-      <c r="BJ1" t="inlineStr">
+      <c r="BK1" t="inlineStr">
         <is>
           <t>rank</t>
         </is>
       </c>
-      <c r="BK1" t="inlineStr">
+      <c r="BL1" t="inlineStr">
         <is>
           <t>categories</t>
         </is>
       </c>
-      <c r="BL1" t="inlineStr">
+      <c r="BM1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
@@ -3501,7 +3359,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AL1"/>
+  <dimension ref="A1:AM1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3512,190 +3370,195 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>syntax</t>
+          <t>alias</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>interpolated</t>
+          <t>maximum_cardinality</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>partial_match</t>
+          <t>minimum_cardinality</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>exact_cardinality</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>extensions</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>annotations</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>alt_descriptions</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>deprecated</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>todos</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>comments</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>examples</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>in_subset</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>from_schema</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>imported_from</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>source</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>in_language</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>deprecated element has exact replacement</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>deprecated element has possible replacement</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>aliases</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>structured_aliases</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>mappings</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>exact mappings</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>close mappings</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>related mappings</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>narrow mappings</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>broad mappings</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>created_by</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>contributors</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>created_on</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>last_updated_on</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>modified_by</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>rank</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>categories</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
@@ -3723,17 +3586,17 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>import_from</t>
+          <t>syntax</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>import_as</t>
+          <t>interpolated</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>import_map</t>
+          <t>partial_match</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -3923,7 +3786,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:AL1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3934,12 +3797,192 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>setting_key</t>
+          <t>import_from</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>setting_value</t>
+          <t>import_as</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>import_map</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>extensions</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>annotations</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>alt_descriptions</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>deprecated</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>todos</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>notes</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>examples</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>in_subset</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>from_schema</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>imported_from</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>in_language</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>see_also</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>deprecated element has exact replacement</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>deprecated element has possible replacement</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>aliases</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>structured_aliases</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>mappings</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>exact mappings</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>close mappings</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>related mappings</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>narrow mappings</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>broad mappings</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>created_by</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>contributors</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>created_on</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>last_updated_on</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>modified_by</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>categories</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>keywords</t>
         </is>
       </c>
     </row>
@@ -3965,12 +4008,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>prefix_prefix</t>
+          <t>setting_key</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>prefix_reference</t>
+          <t>setting_value</t>
         </is>
       </c>
     </row>
@@ -3996,12 +4039,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>local_name_source</t>
+          <t>prefix_prefix</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>local_name_value</t>
+          <t>prefix_reference</t>
         </is>
       </c>
     </row>
@@ -4011,6 +4054,37 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>local_name_source</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>local_name_value</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4046,7 +4120,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4077,7 +4151,238 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AP1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>meaning</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>unit</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>instantiates</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>implements</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>is_a</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>mixins</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>extensions</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>annotations</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>alt_descriptions</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>deprecated</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>todos</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>notes</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>examples</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>in_subset</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>from_schema</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>imported_from</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>in_language</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>see_also</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>deprecated element has exact replacement</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>deprecated element has possible replacement</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>aliases</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>structured_aliases</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>mappings</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>exact mappings</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>close mappings</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>related mappings</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>narrow mappings</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>broad mappings</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>created_by</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>contributors</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>created_on</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>last_updated_on</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>modified_by</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>categories</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>keywords</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4094,34 +4399,34 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>unique_key_name</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>unique_key_slots</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>consider_nulls_inequal</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>extensions</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>annotations</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>description</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>meaning</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>unit</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>extensions</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>annotations</t>
-        </is>
-      </c>
       <c r="G1" t="inlineStr">
         <is>
           <t>alt_descriptions</t>
@@ -4280,278 +4585,6 @@
       <c r="AL1" t="inlineStr">
         <is>
           <t>keywords</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AL1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>unique_key_name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>unique_key_slots</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>consider_nulls_inequal</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>extensions</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>annotations</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>alt_descriptions</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>deprecated</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>todos</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>notes</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>comments</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>examples</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>in_subset</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>from_schema</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>imported_from</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>source</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>in_language</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>see_also</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>deprecated element has exact replacement</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>deprecated element has possible replacement</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>aliases</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>structured_aliases</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>mappings</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>exact mappings</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>close mappings</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>related mappings</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>narrow mappings</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>broad mappings</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>created_by</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>contributors</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>created_on</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>last_updated_on</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>modified_by</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>status</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>rank</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>categories</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>keywords</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>symbol</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>abbreviation</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>descriptive_name</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>exact mappings</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>ucum_code</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>derivation</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>has_quantity_kind</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>iec61360code</t>
         </is>
       </c>
     </row>
@@ -4652,6 +4685,309 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:AL1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>framework_key</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>mapped_type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>string_serialization</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>extensions</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>annotations</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>alt_descriptions</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>deprecated</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>todos</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>notes</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>examples</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>in_subset</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>from_schema</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>imported_from</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>in_language</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>see_also</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>deprecated element has exact replacement</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>deprecated element has possible replacement</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>aliases</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>structured_aliases</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>mappings</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>exact mappings</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>close mappings</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>related mappings</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>narrow mappings</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>broad mappings</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>created_by</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>contributors</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>created_on</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>last_updated_on</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>modified_by</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>categories</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>keywords</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>allowed</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>range_expression</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>symbol</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>abbreviation</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>descriptive_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>exact mappings</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>ucum_code</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>derivation</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>has_quantity_kind</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>iec61360code</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4687,7 +5023,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4705,7 +5041,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -5807,7 +6143,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:AM1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5818,16 +6154,209 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>identifier_pattern</t>
+          <t>range</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>source_ontology</t>
+          <t>obligation_level</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>binds_value_of</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>pv_formula</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>extensions</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>annotations</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>alt_descriptions</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>deprecated</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>todos</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>notes</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>examples</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>in_subset</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>from_schema</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>imported_from</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>in_language</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>see_also</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>deprecated element has exact replacement</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>deprecated element has possible replacement</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>aliases</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>structured_aliases</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>mappings</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>exact mappings</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>close mappings</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>related mappings</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>narrow mappings</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>broad mappings</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>created_by</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>contributors</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>created_on</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>last_updated_on</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>modified_by</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>categories</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>keywords</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"REQUIRED,RECOMMENDED,OPTIONAL,EXAMPLE,DISCOURAGED"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"CODE,CURIE,URI,FHIR_CODING,LABEL"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>